<commit_message>
UDP now bundles Packets
UDP now sends all packets together in one byte block, rather than attempting to send each packet individually which was causing issues with more than 10-20 objects.
</commit_message>
<xml_diff>
--- a/Tests.xlsx
+++ b/Tests.xlsx
@@ -8,9 +8,9 @@
       <x15ac:absPath xmlns:x15ac="http://schemas.microsoft.com/office/spreadsheetml/2010/11/ac" url="C:\Users\Charz\Documents\Unity\GTRP\"/>
     </mc:Choice>
   </mc:AlternateContent>
-  <xr:revisionPtr revIDLastSave="0" documentId="13_ncr:1_{8140093A-B6C3-44EF-A391-8E51A6D85621}" xr6:coauthVersionLast="47" xr6:coauthVersionMax="47" xr10:uidLastSave="{00000000-0000-0000-0000-000000000000}"/>
+  <xr:revisionPtr revIDLastSave="0" documentId="13_ncr:1_{94B38AC0-09D7-4F33-8908-AEBFF3D9A2AC}" xr6:coauthVersionLast="47" xr6:coauthVersionMax="47" xr10:uidLastSave="{00000000-0000-0000-0000-000000000000}"/>
   <bookViews>
-    <workbookView xWindow="-120" yWindow="-120" windowWidth="29040" windowHeight="15840" activeTab="1" xr2:uid="{00000000-000D-0000-FFFF-FFFF00000000}"/>
+    <workbookView xWindow="-120" yWindow="-120" windowWidth="29040" windowHeight="15840" xr2:uid="{00000000-000D-0000-FFFF-FFFF00000000}"/>
   </bookViews>
   <sheets>
     <sheet name="Bandwidth Tests" sheetId="1" r:id="rId1"/>
@@ -34,7 +34,7 @@
 </file>
 
 <file path=xl/sharedStrings.xml><?xml version="1.0" encoding="utf-8"?>
-<sst xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" count="8" uniqueCount="8">
+<sst xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" count="11" uniqueCount="10">
   <si>
     <t>Time (s)</t>
   </si>
@@ -58,6 +58,12 @@
   </si>
   <si>
     <t>fps</t>
+  </si>
+  <si>
+    <t>API</t>
+  </si>
+  <si>
+    <t>Bundled Optimised</t>
   </si>
 </sst>
 </file>
@@ -541,8 +547,11 @@
     <xf numFmtId="0" fontId="1" fillId="31" borderId="0" applyNumberFormat="0" applyBorder="0" applyAlignment="0" applyProtection="0"/>
     <xf numFmtId="0" fontId="1" fillId="32" borderId="0" applyNumberFormat="0" applyBorder="0" applyAlignment="0" applyProtection="0"/>
   </cellStyleXfs>
-  <cellXfs count="1">
+  <cellXfs count="2">
     <xf numFmtId="0" fontId="0" fillId="0" borderId="0" xfId="0"/>
+    <xf numFmtId="0" fontId="0" fillId="0" borderId="0" xfId="0" applyAlignment="1">
+      <alignment horizontal="center"/>
+    </xf>
   </cellXfs>
   <cellStyles count="42">
     <cellStyle name="20% - Accent1" xfId="19" builtinId="30" customBuiltin="1"/>
@@ -2629,6 +2638,357 @@
           <c:extLst>
             <c:ext xmlns:c16="http://schemas.microsoft.com/office/drawing/2014/chart" uri="{C3380CC4-5D6E-409C-BE32-E72D297353CC}">
               <c16:uniqueId val="{00000003-B447-4D8F-833C-B944BC5FF362}"/>
+            </c:ext>
+          </c:extLst>
+        </c:ser>
+        <c:ser>
+          <c:idx val="0"/>
+          <c:order val="3"/>
+          <c:tx>
+            <c:strRef>
+              <c:f>'Bandwidth Tests'!$E$1:$E$2</c:f>
+              <c:strCache>
+                <c:ptCount val="2"/>
+                <c:pt idx="0">
+                  <c:v>Bytes read by</c:v>
+                </c:pt>
+                <c:pt idx="1">
+                  <c:v>Bundled Optimised</c:v>
+                </c:pt>
+              </c:strCache>
+            </c:strRef>
+          </c:tx>
+          <c:spPr>
+            <a:ln w="28575" cap="rnd">
+              <a:solidFill>
+                <a:schemeClr val="accent1"/>
+              </a:solidFill>
+              <a:round/>
+            </a:ln>
+            <a:effectLst/>
+          </c:spPr>
+          <c:marker>
+            <c:symbol val="none"/>
+          </c:marker>
+          <c:val>
+            <c:numRef>
+              <c:f>'Bandwidth Tests'!$E$3:$E$108</c:f>
+              <c:numCache>
+                <c:formatCode>General</c:formatCode>
+                <c:ptCount val="106"/>
+                <c:pt idx="4">
+                  <c:v>0</c:v>
+                </c:pt>
+                <c:pt idx="5">
+                  <c:v>0</c:v>
+                </c:pt>
+                <c:pt idx="6">
+                  <c:v>1051</c:v>
+                </c:pt>
+                <c:pt idx="7">
+                  <c:v>0</c:v>
+                </c:pt>
+                <c:pt idx="8">
+                  <c:v>0</c:v>
+                </c:pt>
+                <c:pt idx="9">
+                  <c:v>555</c:v>
+                </c:pt>
+                <c:pt idx="10">
+                  <c:v>1235</c:v>
+                </c:pt>
+                <c:pt idx="11">
+                  <c:v>1825</c:v>
+                </c:pt>
+                <c:pt idx="12">
+                  <c:v>2588</c:v>
+                </c:pt>
+                <c:pt idx="13">
+                  <c:v>3079</c:v>
+                </c:pt>
+                <c:pt idx="14">
+                  <c:v>3211</c:v>
+                </c:pt>
+                <c:pt idx="15">
+                  <c:v>3620</c:v>
+                </c:pt>
+                <c:pt idx="16">
+                  <c:v>3755</c:v>
+                </c:pt>
+                <c:pt idx="17">
+                  <c:v>4260</c:v>
+                </c:pt>
+                <c:pt idx="18">
+                  <c:v>4363</c:v>
+                </c:pt>
+                <c:pt idx="19">
+                  <c:v>4916</c:v>
+                </c:pt>
+                <c:pt idx="20">
+                  <c:v>4731</c:v>
+                </c:pt>
+                <c:pt idx="21">
+                  <c:v>5172</c:v>
+                </c:pt>
+                <c:pt idx="22">
+                  <c:v>5139</c:v>
+                </c:pt>
+                <c:pt idx="23">
+                  <c:v>5367</c:v>
+                </c:pt>
+                <c:pt idx="24">
+                  <c:v>5892</c:v>
+                </c:pt>
+                <c:pt idx="25">
+                  <c:v>5823</c:v>
+                </c:pt>
+                <c:pt idx="26">
+                  <c:v>6180</c:v>
+                </c:pt>
+                <c:pt idx="27">
+                  <c:v>5871</c:v>
+                </c:pt>
+                <c:pt idx="28">
+                  <c:v>5871</c:v>
+                </c:pt>
+                <c:pt idx="29">
+                  <c:v>6180</c:v>
+                </c:pt>
+                <c:pt idx="30">
+                  <c:v>5871</c:v>
+                </c:pt>
+                <c:pt idx="31">
+                  <c:v>5871</c:v>
+                </c:pt>
+                <c:pt idx="32">
+                  <c:v>6180</c:v>
+                </c:pt>
+                <c:pt idx="33">
+                  <c:v>5871</c:v>
+                </c:pt>
+                <c:pt idx="34">
+                  <c:v>6180</c:v>
+                </c:pt>
+                <c:pt idx="35">
+                  <c:v>5871</c:v>
+                </c:pt>
+                <c:pt idx="36">
+                  <c:v>5871</c:v>
+                </c:pt>
+                <c:pt idx="37">
+                  <c:v>6180</c:v>
+                </c:pt>
+                <c:pt idx="38">
+                  <c:v>5871</c:v>
+                </c:pt>
+                <c:pt idx="39">
+                  <c:v>6180</c:v>
+                </c:pt>
+                <c:pt idx="40">
+                  <c:v>5871</c:v>
+                </c:pt>
+                <c:pt idx="41">
+                  <c:v>5871</c:v>
+                </c:pt>
+                <c:pt idx="42">
+                  <c:v>6180</c:v>
+                </c:pt>
+                <c:pt idx="43">
+                  <c:v>5871</c:v>
+                </c:pt>
+                <c:pt idx="44">
+                  <c:v>5871</c:v>
+                </c:pt>
+                <c:pt idx="45">
+                  <c:v>6180</c:v>
+                </c:pt>
+                <c:pt idx="46">
+                  <c:v>5871</c:v>
+                </c:pt>
+                <c:pt idx="47">
+                  <c:v>6180</c:v>
+                </c:pt>
+                <c:pt idx="48">
+                  <c:v>5871</c:v>
+                </c:pt>
+                <c:pt idx="49">
+                  <c:v>6180</c:v>
+                </c:pt>
+                <c:pt idx="50">
+                  <c:v>5871</c:v>
+                </c:pt>
+                <c:pt idx="51">
+                  <c:v>6180</c:v>
+                </c:pt>
+                <c:pt idx="52">
+                  <c:v>5871</c:v>
+                </c:pt>
+                <c:pt idx="53">
+                  <c:v>5871</c:v>
+                </c:pt>
+                <c:pt idx="54">
+                  <c:v>6180</c:v>
+                </c:pt>
+                <c:pt idx="55">
+                  <c:v>5871</c:v>
+                </c:pt>
+                <c:pt idx="56">
+                  <c:v>6180</c:v>
+                </c:pt>
+                <c:pt idx="57">
+                  <c:v>5871</c:v>
+                </c:pt>
+                <c:pt idx="58">
+                  <c:v>6180</c:v>
+                </c:pt>
+                <c:pt idx="59">
+                  <c:v>5871</c:v>
+                </c:pt>
+                <c:pt idx="60">
+                  <c:v>5871</c:v>
+                </c:pt>
+                <c:pt idx="61">
+                  <c:v>6180</c:v>
+                </c:pt>
+                <c:pt idx="62">
+                  <c:v>5871</c:v>
+                </c:pt>
+                <c:pt idx="63">
+                  <c:v>6180</c:v>
+                </c:pt>
+                <c:pt idx="64">
+                  <c:v>5871</c:v>
+                </c:pt>
+                <c:pt idx="65">
+                  <c:v>6180</c:v>
+                </c:pt>
+                <c:pt idx="66">
+                  <c:v>5871</c:v>
+                </c:pt>
+                <c:pt idx="67">
+                  <c:v>5871</c:v>
+                </c:pt>
+                <c:pt idx="68">
+                  <c:v>6180</c:v>
+                </c:pt>
+                <c:pt idx="69">
+                  <c:v>5871</c:v>
+                </c:pt>
+                <c:pt idx="70">
+                  <c:v>6180</c:v>
+                </c:pt>
+                <c:pt idx="71">
+                  <c:v>5871</c:v>
+                </c:pt>
+                <c:pt idx="72">
+                  <c:v>5871</c:v>
+                </c:pt>
+                <c:pt idx="73">
+                  <c:v>6180</c:v>
+                </c:pt>
+                <c:pt idx="74">
+                  <c:v>5871</c:v>
+                </c:pt>
+                <c:pt idx="75">
+                  <c:v>6180</c:v>
+                </c:pt>
+                <c:pt idx="76">
+                  <c:v>5871</c:v>
+                </c:pt>
+                <c:pt idx="77">
+                  <c:v>5871</c:v>
+                </c:pt>
+                <c:pt idx="78">
+                  <c:v>6180</c:v>
+                </c:pt>
+                <c:pt idx="79">
+                  <c:v>5871</c:v>
+                </c:pt>
+                <c:pt idx="80">
+                  <c:v>6180</c:v>
+                </c:pt>
+                <c:pt idx="81">
+                  <c:v>5871</c:v>
+                </c:pt>
+                <c:pt idx="82">
+                  <c:v>5871</c:v>
+                </c:pt>
+                <c:pt idx="83">
+                  <c:v>6180</c:v>
+                </c:pt>
+                <c:pt idx="84">
+                  <c:v>5871</c:v>
+                </c:pt>
+                <c:pt idx="85">
+                  <c:v>6180</c:v>
+                </c:pt>
+                <c:pt idx="86">
+                  <c:v>5871</c:v>
+                </c:pt>
+                <c:pt idx="87">
+                  <c:v>5871</c:v>
+                </c:pt>
+                <c:pt idx="88">
+                  <c:v>6180</c:v>
+                </c:pt>
+                <c:pt idx="89">
+                  <c:v>5871</c:v>
+                </c:pt>
+                <c:pt idx="90">
+                  <c:v>6180</c:v>
+                </c:pt>
+                <c:pt idx="91">
+                  <c:v>5871</c:v>
+                </c:pt>
+                <c:pt idx="92">
+                  <c:v>5871</c:v>
+                </c:pt>
+                <c:pt idx="93">
+                  <c:v>6180</c:v>
+                </c:pt>
+                <c:pt idx="94">
+                  <c:v>5871</c:v>
+                </c:pt>
+                <c:pt idx="95">
+                  <c:v>5871</c:v>
+                </c:pt>
+                <c:pt idx="96">
+                  <c:v>6180</c:v>
+                </c:pt>
+                <c:pt idx="97">
+                  <c:v>5871</c:v>
+                </c:pt>
+                <c:pt idx="98">
+                  <c:v>6180</c:v>
+                </c:pt>
+                <c:pt idx="99">
+                  <c:v>5871</c:v>
+                </c:pt>
+                <c:pt idx="100">
+                  <c:v>5871</c:v>
+                </c:pt>
+                <c:pt idx="101">
+                  <c:v>6180</c:v>
+                </c:pt>
+                <c:pt idx="102">
+                  <c:v>5871</c:v>
+                </c:pt>
+                <c:pt idx="103">
+                  <c:v>6180</c:v>
+                </c:pt>
+                <c:pt idx="104">
+                  <c:v>5871</c:v>
+                </c:pt>
+                <c:pt idx="105">
+                  <c:v>6180</c:v>
+                </c:pt>
+              </c:numCache>
+            </c:numRef>
+          </c:val>
+          <c:smooth val="0"/>
+          <c:extLst>
+            <c:ext xmlns:c16="http://schemas.microsoft.com/office/drawing/2014/chart" uri="{C3380CC4-5D6E-409C-BE32-E72D297353CC}">
+              <c16:uniqueId val="{00000002-B2C7-40D3-BA92-2C04CB1C27A8}"/>
             </c:ext>
           </c:extLst>
         </c:ser>
@@ -3504,16 +3864,16 @@
 <xdr:wsDr xmlns:xdr="http://schemas.openxmlformats.org/drawingml/2006/spreadsheetDrawing" xmlns:a="http://schemas.openxmlformats.org/drawingml/2006/main">
   <xdr:twoCellAnchor>
     <xdr:from>
-      <xdr:col>7</xdr:col>
-      <xdr:colOff>114300</xdr:colOff>
-      <xdr:row>72</xdr:row>
-      <xdr:rowOff>157162</xdr:rowOff>
+      <xdr:col>6</xdr:col>
+      <xdr:colOff>9525</xdr:colOff>
+      <xdr:row>1</xdr:row>
+      <xdr:rowOff>52387</xdr:rowOff>
     </xdr:from>
     <xdr:to>
-      <xdr:col>14</xdr:col>
-      <xdr:colOff>419100</xdr:colOff>
-      <xdr:row>87</xdr:row>
-      <xdr:rowOff>42862</xdr:rowOff>
+      <xdr:col>13</xdr:col>
+      <xdr:colOff>314325</xdr:colOff>
+      <xdr:row>15</xdr:row>
+      <xdr:rowOff>128587</xdr:rowOff>
     </xdr:to>
     <xdr:graphicFrame macro="">
       <xdr:nvGraphicFramePr>
@@ -3838,23 +4198,30 @@
 
 <file path=xl/worksheets/sheet1.xml><?xml version="1.0" encoding="utf-8"?>
 <worksheet xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" xmlns:r="http://schemas.openxmlformats.org/officeDocument/2006/relationships" xmlns:mc="http://schemas.openxmlformats.org/markup-compatibility/2006" xmlns:x14ac="http://schemas.microsoft.com/office/spreadsheetml/2009/9/ac" xmlns:xr="http://schemas.microsoft.com/office/spreadsheetml/2014/revision" xmlns:xr2="http://schemas.microsoft.com/office/spreadsheetml/2015/revision2" xmlns:xr3="http://schemas.microsoft.com/office/spreadsheetml/2016/revision3" mc:Ignorable="x14ac xr xr2 xr3" xr:uid="{00000000-0001-0000-0000-000000000000}">
-  <dimension ref="A1:D148"/>
+  <dimension ref="A1:E148"/>
   <sheetViews>
-    <sheetView topLeftCell="A60" workbookViewId="0">
-      <selection activeCell="F77" sqref="F77"/>
+    <sheetView tabSelected="1" workbookViewId="0">
+      <selection activeCell="J28" sqref="J28"/>
     </sheetView>
   </sheetViews>
   <sheetFormatPr defaultRowHeight="15" x14ac:dyDescent="0.25"/>
+  <cols>
+    <col min="4" max="4" width="10.28515625" bestFit="1" customWidth="1"/>
+    <col min="5" max="5" width="18.42578125" bestFit="1" customWidth="1"/>
+  </cols>
   <sheetData>
-    <row r="1" spans="1:4" x14ac:dyDescent="0.25">
+    <row r="1" spans="1:5" x14ac:dyDescent="0.25">
       <c r="A1" t="s">
         <v>0</v>
       </c>
-      <c r="B1" t="s">
+      <c r="B1" s="1" t="s">
         <v>1</v>
       </c>
-    </row>
-    <row r="2" spans="1:4" x14ac:dyDescent="0.25">
+      <c r="C1" s="1"/>
+      <c r="D1" s="1"/>
+      <c r="E1" s="1"/>
+    </row>
+    <row r="2" spans="1:5" x14ac:dyDescent="0.25">
       <c r="B2" t="s">
         <v>2</v>
       </c>
@@ -3864,8 +4231,11 @@
       <c r="D2" t="s">
         <v>4</v>
       </c>
-    </row>
-    <row r="3" spans="1:4" x14ac:dyDescent="0.25">
+      <c r="E2" t="s">
+        <v>9</v>
+      </c>
+    </row>
+    <row r="3" spans="1:5" x14ac:dyDescent="0.25">
       <c r="A3">
         <v>-5</v>
       </c>
@@ -3873,7 +4243,7 @@
         <v>0</v>
       </c>
     </row>
-    <row r="4" spans="1:4" x14ac:dyDescent="0.25">
+    <row r="4" spans="1:5" x14ac:dyDescent="0.25">
       <c r="A4">
         <v>-4</v>
       </c>
@@ -3881,7 +4251,7 @@
         <v>0</v>
       </c>
     </row>
-    <row r="5" spans="1:4" x14ac:dyDescent="0.25">
+    <row r="5" spans="1:5" x14ac:dyDescent="0.25">
       <c r="A5">
         <v>-3</v>
       </c>
@@ -3889,7 +4259,7 @@
         <v>0</v>
       </c>
     </row>
-    <row r="6" spans="1:4" x14ac:dyDescent="0.25">
+    <row r="6" spans="1:5" x14ac:dyDescent="0.25">
       <c r="A6">
         <v>-2</v>
       </c>
@@ -3897,7 +4267,7 @@
         <v>0</v>
       </c>
     </row>
-    <row r="7" spans="1:4" x14ac:dyDescent="0.25">
+    <row r="7" spans="1:5" x14ac:dyDescent="0.25">
       <c r="A7">
         <v>-1</v>
       </c>
@@ -3907,8 +4277,11 @@
       <c r="D7">
         <v>0</v>
       </c>
-    </row>
-    <row r="8" spans="1:4" x14ac:dyDescent="0.25">
+      <c r="E7">
+        <v>0</v>
+      </c>
+    </row>
+    <row r="8" spans="1:5" x14ac:dyDescent="0.25">
       <c r="A8">
         <v>0</v>
       </c>
@@ -3918,8 +4291,11 @@
       <c r="D8">
         <v>0</v>
       </c>
-    </row>
-    <row r="9" spans="1:4" x14ac:dyDescent="0.25">
+      <c r="E8">
+        <v>0</v>
+      </c>
+    </row>
+    <row r="9" spans="1:5" x14ac:dyDescent="0.25">
       <c r="A9">
         <v>1</v>
       </c>
@@ -3929,8 +4305,11 @@
       <c r="D9">
         <v>774</v>
       </c>
-    </row>
-    <row r="10" spans="1:4" x14ac:dyDescent="0.25">
+      <c r="E9">
+        <v>1051</v>
+      </c>
+    </row>
+    <row r="10" spans="1:5" x14ac:dyDescent="0.25">
       <c r="A10">
         <v>2</v>
       </c>
@@ -3940,8 +4319,11 @@
       <c r="D10">
         <v>277</v>
       </c>
-    </row>
-    <row r="11" spans="1:4" x14ac:dyDescent="0.25">
+      <c r="E10">
+        <v>0</v>
+      </c>
+    </row>
+    <row r="11" spans="1:5" x14ac:dyDescent="0.25">
       <c r="A11">
         <v>3</v>
       </c>
@@ -3951,8 +4333,11 @@
       <c r="D11">
         <v>0</v>
       </c>
-    </row>
-    <row r="12" spans="1:4" x14ac:dyDescent="0.25">
+      <c r="E11">
+        <v>0</v>
+      </c>
+    </row>
+    <row r="12" spans="1:5" x14ac:dyDescent="0.25">
       <c r="A12">
         <v>4</v>
       </c>
@@ -3962,8 +4347,11 @@
       <c r="D12">
         <v>406</v>
       </c>
-    </row>
-    <row r="13" spans="1:4" x14ac:dyDescent="0.25">
+      <c r="E12">
+        <v>555</v>
+      </c>
+    </row>
+    <row r="13" spans="1:5" x14ac:dyDescent="0.25">
       <c r="A13">
         <v>5</v>
       </c>
@@ -3973,8 +4361,11 @@
       <c r="D13">
         <v>986</v>
       </c>
-    </row>
-    <row r="14" spans="1:4" x14ac:dyDescent="0.25">
+      <c r="E13">
+        <v>1235</v>
+      </c>
+    </row>
+    <row r="14" spans="1:5" x14ac:dyDescent="0.25">
       <c r="A14">
         <v>6</v>
       </c>
@@ -3984,8 +4375,11 @@
       <c r="D14">
         <v>1595</v>
       </c>
-    </row>
-    <row r="15" spans="1:4" x14ac:dyDescent="0.25">
+      <c r="E14">
+        <v>1825</v>
+      </c>
+    </row>
+    <row r="15" spans="1:5" x14ac:dyDescent="0.25">
       <c r="A15">
         <v>7</v>
       </c>
@@ -3995,8 +4389,11 @@
       <c r="D15">
         <v>2175</v>
       </c>
-    </row>
-    <row r="16" spans="1:4" x14ac:dyDescent="0.25">
+      <c r="E15">
+        <v>2588</v>
+      </c>
+    </row>
+    <row r="16" spans="1:5" x14ac:dyDescent="0.25">
       <c r="A16">
         <v>8</v>
       </c>
@@ -4006,8 +4403,11 @@
       <c r="D16">
         <v>2755</v>
       </c>
-    </row>
-    <row r="17" spans="1:4" x14ac:dyDescent="0.25">
+      <c r="E16">
+        <v>3079</v>
+      </c>
+    </row>
+    <row r="17" spans="1:5" x14ac:dyDescent="0.25">
       <c r="A17">
         <v>9</v>
       </c>
@@ -4017,8 +4417,11 @@
       <c r="D17">
         <v>2842</v>
       </c>
-    </row>
-    <row r="18" spans="1:4" x14ac:dyDescent="0.25">
+      <c r="E17">
+        <v>3211</v>
+      </c>
+    </row>
+    <row r="18" spans="1:5" x14ac:dyDescent="0.25">
       <c r="A18">
         <v>10</v>
       </c>
@@ -4028,8 +4431,11 @@
       <c r="D18">
         <v>3037</v>
       </c>
-    </row>
-    <row r="19" spans="1:4" x14ac:dyDescent="0.25">
+      <c r="E18">
+        <v>3620</v>
+      </c>
+    </row>
+    <row r="19" spans="1:5" x14ac:dyDescent="0.25">
       <c r="A19">
         <v>11</v>
       </c>
@@ -4039,8 +4445,11 @@
       <c r="D19">
         <v>3460</v>
       </c>
-    </row>
-    <row r="20" spans="1:4" x14ac:dyDescent="0.25">
+      <c r="E19">
+        <v>3755</v>
+      </c>
+    </row>
+    <row r="20" spans="1:5" x14ac:dyDescent="0.25">
       <c r="A20">
         <v>12</v>
       </c>
@@ -4050,8 +4459,11 @@
       <c r="D20">
         <v>3780</v>
       </c>
-    </row>
-    <row r="21" spans="1:4" x14ac:dyDescent="0.25">
+      <c r="E20">
+        <v>4260</v>
+      </c>
+    </row>
+    <row r="21" spans="1:5" x14ac:dyDescent="0.25">
       <c r="A21">
         <v>13</v>
       </c>
@@ -4061,8 +4473,11 @@
       <c r="D21">
         <v>4100</v>
       </c>
-    </row>
-    <row r="22" spans="1:4" x14ac:dyDescent="0.25">
+      <c r="E21">
+        <v>4363</v>
+      </c>
+    </row>
+    <row r="22" spans="1:5" x14ac:dyDescent="0.25">
       <c r="A22">
         <v>14</v>
       </c>
@@ -4072,8 +4487,11 @@
       <c r="D22">
         <v>4330</v>
       </c>
-    </row>
-    <row r="23" spans="1:4" x14ac:dyDescent="0.25">
+      <c r="E22">
+        <v>4916</v>
+      </c>
+    </row>
+    <row r="23" spans="1:5" x14ac:dyDescent="0.25">
       <c r="A23">
         <v>15</v>
       </c>
@@ -4083,8 +4501,11 @@
       <c r="D23">
         <v>4365</v>
       </c>
-    </row>
-    <row r="24" spans="1:4" x14ac:dyDescent="0.25">
+      <c r="E23">
+        <v>4731</v>
+      </c>
+    </row>
+    <row r="24" spans="1:5" x14ac:dyDescent="0.25">
       <c r="A24">
         <v>16</v>
       </c>
@@ -4094,8 +4515,11 @@
       <c r="D24">
         <v>4680</v>
       </c>
-    </row>
-    <row r="25" spans="1:4" x14ac:dyDescent="0.25">
+      <c r="E24">
+        <v>5172</v>
+      </c>
+    </row>
+    <row r="25" spans="1:5" x14ac:dyDescent="0.25">
       <c r="A25">
         <v>17</v>
       </c>
@@ -4105,8 +4529,11 @@
       <c r="D25">
         <v>4920</v>
       </c>
-    </row>
-    <row r="26" spans="1:4" x14ac:dyDescent="0.25">
+      <c r="E25">
+        <v>5139</v>
+      </c>
+    </row>
+    <row r="26" spans="1:5" x14ac:dyDescent="0.25">
       <c r="A26">
         <v>18</v>
       </c>
@@ -4116,8 +4543,11 @@
       <c r="D26">
         <v>5160</v>
       </c>
-    </row>
-    <row r="27" spans="1:4" x14ac:dyDescent="0.25">
+      <c r="E26">
+        <v>5367</v>
+      </c>
+    </row>
+    <row r="27" spans="1:5" x14ac:dyDescent="0.25">
       <c r="A27">
         <v>19</v>
       </c>
@@ -4127,8 +4557,11 @@
       <c r="D27">
         <v>5400</v>
       </c>
-    </row>
-    <row r="28" spans="1:4" x14ac:dyDescent="0.25">
+      <c r="E27">
+        <v>5892</v>
+      </c>
+    </row>
+    <row r="28" spans="1:5" x14ac:dyDescent="0.25">
       <c r="A28">
         <v>20</v>
       </c>
@@ -4138,8 +4571,11 @@
       <c r="D28">
         <v>5640</v>
       </c>
-    </row>
-    <row r="29" spans="1:4" x14ac:dyDescent="0.25">
+      <c r="E28">
+        <v>5823</v>
+      </c>
+    </row>
+    <row r="29" spans="1:5" x14ac:dyDescent="0.25">
       <c r="A29">
         <v>21</v>
       </c>
@@ -4149,8 +4585,11 @@
       <c r="D29">
         <v>5415</v>
       </c>
-    </row>
-    <row r="30" spans="1:4" x14ac:dyDescent="0.25">
+      <c r="E29">
+        <v>6180</v>
+      </c>
+    </row>
+    <row r="30" spans="1:5" x14ac:dyDescent="0.25">
       <c r="A30">
         <v>22</v>
       </c>
@@ -4160,8 +4599,11 @@
       <c r="D30">
         <v>5700</v>
       </c>
-    </row>
-    <row r="31" spans="1:4" x14ac:dyDescent="0.25">
+      <c r="E30">
+        <v>5871</v>
+      </c>
+    </row>
+    <row r="31" spans="1:5" x14ac:dyDescent="0.25">
       <c r="A31">
         <v>23</v>
       </c>
@@ -4171,8 +4613,11 @@
       <c r="D31">
         <v>5700</v>
       </c>
-    </row>
-    <row r="32" spans="1:4" x14ac:dyDescent="0.25">
+      <c r="E31">
+        <v>5871</v>
+      </c>
+    </row>
+    <row r="32" spans="1:5" x14ac:dyDescent="0.25">
       <c r="A32">
         <v>24</v>
       </c>
@@ -4182,8 +4627,11 @@
       <c r="D32">
         <v>5700</v>
       </c>
-    </row>
-    <row r="33" spans="1:4" x14ac:dyDescent="0.25">
+      <c r="E32">
+        <v>6180</v>
+      </c>
+    </row>
+    <row r="33" spans="1:5" x14ac:dyDescent="0.25">
       <c r="A33">
         <v>25</v>
       </c>
@@ -4193,8 +4641,11 @@
       <c r="D33">
         <v>5700</v>
       </c>
-    </row>
-    <row r="34" spans="1:4" x14ac:dyDescent="0.25">
+      <c r="E33">
+        <v>5871</v>
+      </c>
+    </row>
+    <row r="34" spans="1:5" x14ac:dyDescent="0.25">
       <c r="A34">
         <v>26</v>
       </c>
@@ -4204,8 +4655,11 @@
       <c r="D34">
         <v>5700</v>
       </c>
-    </row>
-    <row r="35" spans="1:4" x14ac:dyDescent="0.25">
+      <c r="E34">
+        <v>5871</v>
+      </c>
+    </row>
+    <row r="35" spans="1:5" x14ac:dyDescent="0.25">
       <c r="A35">
         <v>27</v>
       </c>
@@ -4215,8 +4669,11 @@
       <c r="D35">
         <v>5415</v>
       </c>
-    </row>
-    <row r="36" spans="1:4" x14ac:dyDescent="0.25">
+      <c r="E35">
+        <v>6180</v>
+      </c>
+    </row>
+    <row r="36" spans="1:5" x14ac:dyDescent="0.25">
       <c r="A36">
         <v>28</v>
       </c>
@@ -4226,8 +4683,11 @@
       <c r="D36">
         <v>5700</v>
       </c>
-    </row>
-    <row r="37" spans="1:4" x14ac:dyDescent="0.25">
+      <c r="E36">
+        <v>5871</v>
+      </c>
+    </row>
+    <row r="37" spans="1:5" x14ac:dyDescent="0.25">
       <c r="A37">
         <v>29</v>
       </c>
@@ -4237,8 +4697,11 @@
       <c r="D37">
         <v>5700</v>
       </c>
-    </row>
-    <row r="38" spans="1:4" x14ac:dyDescent="0.25">
+      <c r="E37">
+        <v>6180</v>
+      </c>
+    </row>
+    <row r="38" spans="1:5" x14ac:dyDescent="0.25">
       <c r="A38">
         <v>30</v>
       </c>
@@ -4248,8 +4711,11 @@
       <c r="D38">
         <v>5700</v>
       </c>
-    </row>
-    <row r="39" spans="1:4" x14ac:dyDescent="0.25">
+      <c r="E38">
+        <v>5871</v>
+      </c>
+    </row>
+    <row r="39" spans="1:5" x14ac:dyDescent="0.25">
       <c r="A39">
         <v>31</v>
       </c>
@@ -4259,8 +4725,11 @@
       <c r="D39">
         <v>5700</v>
       </c>
-    </row>
-    <row r="40" spans="1:4" x14ac:dyDescent="0.25">
+      <c r="E39">
+        <v>5871</v>
+      </c>
+    </row>
+    <row r="40" spans="1:5" x14ac:dyDescent="0.25">
       <c r="A40">
         <v>32</v>
       </c>
@@ -4270,8 +4739,11 @@
       <c r="D40">
         <v>5700</v>
       </c>
-    </row>
-    <row r="41" spans="1:4" x14ac:dyDescent="0.25">
+      <c r="E40">
+        <v>6180</v>
+      </c>
+    </row>
+    <row r="41" spans="1:5" x14ac:dyDescent="0.25">
       <c r="A41">
         <v>33</v>
       </c>
@@ -4281,8 +4753,11 @@
       <c r="D41">
         <v>5529</v>
       </c>
-    </row>
-    <row r="42" spans="1:4" x14ac:dyDescent="0.25">
+      <c r="E41">
+        <v>5871</v>
+      </c>
+    </row>
+    <row r="42" spans="1:5" x14ac:dyDescent="0.25">
       <c r="A42">
         <v>34</v>
       </c>
@@ -4292,8 +4767,11 @@
       <c r="D42">
         <v>5586</v>
       </c>
-    </row>
-    <row r="43" spans="1:4" x14ac:dyDescent="0.25">
+      <c r="E42">
+        <v>6180</v>
+      </c>
+    </row>
+    <row r="43" spans="1:5" x14ac:dyDescent="0.25">
       <c r="A43">
         <v>35</v>
       </c>
@@ -4303,8 +4781,11 @@
       <c r="D43">
         <v>5700</v>
       </c>
-    </row>
-    <row r="44" spans="1:4" x14ac:dyDescent="0.25">
+      <c r="E43">
+        <v>5871</v>
+      </c>
+    </row>
+    <row r="44" spans="1:5" x14ac:dyDescent="0.25">
       <c r="A44">
         <v>36</v>
       </c>
@@ -4314,8 +4795,11 @@
       <c r="D44">
         <v>5700</v>
       </c>
-    </row>
-    <row r="45" spans="1:4" x14ac:dyDescent="0.25">
+      <c r="E44">
+        <v>5871</v>
+      </c>
+    </row>
+    <row r="45" spans="1:5" x14ac:dyDescent="0.25">
       <c r="A45">
         <v>37</v>
       </c>
@@ -4325,8 +4809,11 @@
       <c r="D45">
         <v>5700</v>
       </c>
-    </row>
-    <row r="46" spans="1:4" x14ac:dyDescent="0.25">
+      <c r="E45">
+        <v>6180</v>
+      </c>
+    </row>
+    <row r="46" spans="1:5" x14ac:dyDescent="0.25">
       <c r="A46">
         <v>38</v>
       </c>
@@ -4336,8 +4823,11 @@
       <c r="D46">
         <v>5643</v>
       </c>
-    </row>
-    <row r="47" spans="1:4" x14ac:dyDescent="0.25">
+      <c r="E46">
+        <v>5871</v>
+      </c>
+    </row>
+    <row r="47" spans="1:5" x14ac:dyDescent="0.25">
       <c r="A47">
         <v>39</v>
       </c>
@@ -4347,8 +4837,11 @@
       <c r="D47">
         <v>5472</v>
       </c>
-    </row>
-    <row r="48" spans="1:4" x14ac:dyDescent="0.25">
+      <c r="E47">
+        <v>5871</v>
+      </c>
+    </row>
+    <row r="48" spans="1:5" x14ac:dyDescent="0.25">
       <c r="A48">
         <v>40</v>
       </c>
@@ -4358,8 +4851,11 @@
       <c r="D48">
         <v>5700</v>
       </c>
-    </row>
-    <row r="49" spans="1:4" x14ac:dyDescent="0.25">
+      <c r="E48">
+        <v>6180</v>
+      </c>
+    </row>
+    <row r="49" spans="1:5" x14ac:dyDescent="0.25">
       <c r="A49">
         <v>41</v>
       </c>
@@ -4369,8 +4865,11 @@
       <c r="D49">
         <v>5700</v>
       </c>
-    </row>
-    <row r="50" spans="1:4" x14ac:dyDescent="0.25">
+      <c r="E49">
+        <v>5871</v>
+      </c>
+    </row>
+    <row r="50" spans="1:5" x14ac:dyDescent="0.25">
       <c r="A50">
         <v>42</v>
       </c>
@@ -4380,8 +4879,11 @@
       <c r="D50">
         <v>5700</v>
       </c>
-    </row>
-    <row r="51" spans="1:4" x14ac:dyDescent="0.25">
+      <c r="E50">
+        <v>6180</v>
+      </c>
+    </row>
+    <row r="51" spans="1:5" x14ac:dyDescent="0.25">
       <c r="A51">
         <v>43</v>
       </c>
@@ -4391,8 +4893,11 @@
       <c r="D51">
         <v>5700</v>
       </c>
-    </row>
-    <row r="52" spans="1:4" x14ac:dyDescent="0.25">
+      <c r="E51">
+        <v>5871</v>
+      </c>
+    </row>
+    <row r="52" spans="1:5" x14ac:dyDescent="0.25">
       <c r="A52">
         <v>44</v>
       </c>
@@ -4402,8 +4907,11 @@
       <c r="D52">
         <v>5472</v>
       </c>
-    </row>
-    <row r="53" spans="1:4" x14ac:dyDescent="0.25">
+      <c r="E52">
+        <v>6180</v>
+      </c>
+    </row>
+    <row r="53" spans="1:5" x14ac:dyDescent="0.25">
       <c r="A53">
         <v>45</v>
       </c>
@@ -4413,8 +4921,11 @@
       <c r="D53">
         <v>5643</v>
       </c>
-    </row>
-    <row r="54" spans="1:4" x14ac:dyDescent="0.25">
+      <c r="E53">
+        <v>5871</v>
+      </c>
+    </row>
+    <row r="54" spans="1:5" x14ac:dyDescent="0.25">
       <c r="A54">
         <v>46</v>
       </c>
@@ -4424,8 +4935,11 @@
       <c r="D54">
         <v>5700</v>
       </c>
-    </row>
-    <row r="55" spans="1:4" x14ac:dyDescent="0.25">
+      <c r="E54">
+        <v>6180</v>
+      </c>
+    </row>
+    <row r="55" spans="1:5" x14ac:dyDescent="0.25">
       <c r="A55">
         <v>47</v>
       </c>
@@ -4435,8 +4949,11 @@
       <c r="D55">
         <v>5700</v>
       </c>
-    </row>
-    <row r="56" spans="1:4" x14ac:dyDescent="0.25">
+      <c r="E55">
+        <v>5871</v>
+      </c>
+    </row>
+    <row r="56" spans="1:5" x14ac:dyDescent="0.25">
       <c r="A56">
         <v>48</v>
       </c>
@@ -4446,8 +4963,11 @@
       <c r="D56">
         <v>5700</v>
       </c>
-    </row>
-    <row r="57" spans="1:4" x14ac:dyDescent="0.25">
+      <c r="E56">
+        <v>5871</v>
+      </c>
+    </row>
+    <row r="57" spans="1:5" x14ac:dyDescent="0.25">
       <c r="A57">
         <v>49</v>
       </c>
@@ -4457,8 +4977,11 @@
       <c r="D57">
         <v>5700</v>
       </c>
-    </row>
-    <row r="58" spans="1:4" x14ac:dyDescent="0.25">
+      <c r="E57">
+        <v>6180</v>
+      </c>
+    </row>
+    <row r="58" spans="1:5" x14ac:dyDescent="0.25">
       <c r="A58">
         <v>50</v>
       </c>
@@ -4468,8 +4991,11 @@
       <c r="D58">
         <v>5529</v>
       </c>
-    </row>
-    <row r="59" spans="1:4" x14ac:dyDescent="0.25">
+      <c r="E58">
+        <v>5871</v>
+      </c>
+    </row>
+    <row r="59" spans="1:5" x14ac:dyDescent="0.25">
       <c r="A59">
         <v>51</v>
       </c>
@@ -4479,8 +5005,11 @@
       <c r="D59">
         <v>5586</v>
       </c>
-    </row>
-    <row r="60" spans="1:4" x14ac:dyDescent="0.25">
+      <c r="E59">
+        <v>6180</v>
+      </c>
+    </row>
+    <row r="60" spans="1:5" x14ac:dyDescent="0.25">
       <c r="A60">
         <v>52</v>
       </c>
@@ -4490,8 +5019,11 @@
       <c r="D60">
         <v>5700</v>
       </c>
-    </row>
-    <row r="61" spans="1:4" x14ac:dyDescent="0.25">
+      <c r="E60">
+        <v>5871</v>
+      </c>
+    </row>
+    <row r="61" spans="1:5" x14ac:dyDescent="0.25">
       <c r="A61">
         <v>53</v>
       </c>
@@ -4501,8 +5033,11 @@
       <c r="D61">
         <v>5700</v>
       </c>
-    </row>
-    <row r="62" spans="1:4" x14ac:dyDescent="0.25">
+      <c r="E61">
+        <v>6180</v>
+      </c>
+    </row>
+    <row r="62" spans="1:5" x14ac:dyDescent="0.25">
       <c r="A62">
         <v>54</v>
       </c>
@@ -4512,8 +5047,11 @@
       <c r="D62">
         <v>5700</v>
       </c>
-    </row>
-    <row r="63" spans="1:4" x14ac:dyDescent="0.25">
+      <c r="E62">
+        <v>5871</v>
+      </c>
+    </row>
+    <row r="63" spans="1:5" x14ac:dyDescent="0.25">
       <c r="A63">
         <v>55</v>
       </c>
@@ -4523,8 +5061,11 @@
       <c r="D63">
         <v>5529</v>
       </c>
-    </row>
-    <row r="64" spans="1:4" x14ac:dyDescent="0.25">
+      <c r="E63">
+        <v>5871</v>
+      </c>
+    </row>
+    <row r="64" spans="1:5" x14ac:dyDescent="0.25">
       <c r="A64">
         <v>56</v>
       </c>
@@ -4534,8 +5075,11 @@
       <c r="D64">
         <v>5586</v>
       </c>
-    </row>
-    <row r="65" spans="1:4" x14ac:dyDescent="0.25">
+      <c r="E64">
+        <v>6180</v>
+      </c>
+    </row>
+    <row r="65" spans="1:5" x14ac:dyDescent="0.25">
       <c r="A65">
         <v>57</v>
       </c>
@@ -4545,8 +5089,11 @@
       <c r="D65">
         <v>5700</v>
       </c>
-    </row>
-    <row r="66" spans="1:4" x14ac:dyDescent="0.25">
+      <c r="E65">
+        <v>5871</v>
+      </c>
+    </row>
+    <row r="66" spans="1:5" x14ac:dyDescent="0.25">
       <c r="A66">
         <v>58</v>
       </c>
@@ -4556,8 +5103,11 @@
       <c r="D66">
         <v>5700</v>
       </c>
-    </row>
-    <row r="67" spans="1:4" x14ac:dyDescent="0.25">
+      <c r="E66">
+        <v>6180</v>
+      </c>
+    </row>
+    <row r="67" spans="1:5" x14ac:dyDescent="0.25">
       <c r="A67">
         <v>59</v>
       </c>
@@ -4567,8 +5117,11 @@
       <c r="D67">
         <v>5700</v>
       </c>
-    </row>
-    <row r="68" spans="1:4" x14ac:dyDescent="0.25">
+      <c r="E67">
+        <v>5871</v>
+      </c>
+    </row>
+    <row r="68" spans="1:5" x14ac:dyDescent="0.25">
       <c r="A68">
         <v>60</v>
       </c>
@@ -4578,8 +5131,11 @@
       <c r="D68">
         <v>5700</v>
       </c>
-    </row>
-    <row r="69" spans="1:4" x14ac:dyDescent="0.25">
+      <c r="E68">
+        <v>6180</v>
+      </c>
+    </row>
+    <row r="69" spans="1:5" x14ac:dyDescent="0.25">
       <c r="A69">
         <v>61</v>
       </c>
@@ -4589,8 +5145,11 @@
       <c r="D69">
         <v>5586</v>
       </c>
-    </row>
-    <row r="70" spans="1:4" x14ac:dyDescent="0.25">
+      <c r="E69">
+        <v>5871</v>
+      </c>
+    </row>
+    <row r="70" spans="1:5" x14ac:dyDescent="0.25">
       <c r="A70">
         <v>62</v>
       </c>
@@ -4600,8 +5159,11 @@
       <c r="D70">
         <v>5529</v>
       </c>
-    </row>
-    <row r="71" spans="1:4" x14ac:dyDescent="0.25">
+      <c r="E70">
+        <v>5871</v>
+      </c>
+    </row>
+    <row r="71" spans="1:5" x14ac:dyDescent="0.25">
       <c r="A71">
         <v>63</v>
       </c>
@@ -4611,8 +5173,11 @@
       <c r="D71">
         <v>5700</v>
       </c>
-    </row>
-    <row r="72" spans="1:4" x14ac:dyDescent="0.25">
+      <c r="E71">
+        <v>6180</v>
+      </c>
+    </row>
+    <row r="72" spans="1:5" x14ac:dyDescent="0.25">
       <c r="A72">
         <v>64</v>
       </c>
@@ -4622,8 +5187,11 @@
       <c r="D72">
         <v>5700</v>
       </c>
-    </row>
-    <row r="73" spans="1:4" x14ac:dyDescent="0.25">
+      <c r="E72">
+        <v>5871</v>
+      </c>
+    </row>
+    <row r="73" spans="1:5" x14ac:dyDescent="0.25">
       <c r="A73">
         <v>65</v>
       </c>
@@ -4633,8 +5201,11 @@
       <c r="D73">
         <v>5700</v>
       </c>
-    </row>
-    <row r="74" spans="1:4" x14ac:dyDescent="0.25">
+      <c r="E73">
+        <v>6180</v>
+      </c>
+    </row>
+    <row r="74" spans="1:5" x14ac:dyDescent="0.25">
       <c r="A74">
         <v>66</v>
       </c>
@@ -4644,8 +5215,11 @@
       <c r="D74">
         <v>5700</v>
       </c>
-    </row>
-    <row r="75" spans="1:4" x14ac:dyDescent="0.25">
+      <c r="E74">
+        <v>5871</v>
+      </c>
+    </row>
+    <row r="75" spans="1:5" x14ac:dyDescent="0.25">
       <c r="A75">
         <v>67</v>
       </c>
@@ -4655,8 +5229,11 @@
       <c r="D75">
         <v>5529</v>
       </c>
-    </row>
-    <row r="76" spans="1:4" x14ac:dyDescent="0.25">
+      <c r="E75">
+        <v>5871</v>
+      </c>
+    </row>
+    <row r="76" spans="1:5" x14ac:dyDescent="0.25">
       <c r="A76">
         <v>68</v>
       </c>
@@ -4666,8 +5243,11 @@
       <c r="D76">
         <v>5586</v>
       </c>
-    </row>
-    <row r="77" spans="1:4" x14ac:dyDescent="0.25">
+      <c r="E76">
+        <v>6180</v>
+      </c>
+    </row>
+    <row r="77" spans="1:5" x14ac:dyDescent="0.25">
       <c r="A77">
         <v>69</v>
       </c>
@@ -4677,8 +5257,11 @@
       <c r="D77">
         <v>5700</v>
       </c>
-    </row>
-    <row r="78" spans="1:4" x14ac:dyDescent="0.25">
+      <c r="E77">
+        <v>5871</v>
+      </c>
+    </row>
+    <row r="78" spans="1:5" x14ac:dyDescent="0.25">
       <c r="A78">
         <v>70</v>
       </c>
@@ -4688,8 +5271,11 @@
       <c r="D78">
         <v>5700</v>
       </c>
-    </row>
-    <row r="79" spans="1:4" x14ac:dyDescent="0.25">
+      <c r="E78">
+        <v>6180</v>
+      </c>
+    </row>
+    <row r="79" spans="1:5" x14ac:dyDescent="0.25">
       <c r="A79">
         <v>71</v>
       </c>
@@ -4699,8 +5285,11 @@
       <c r="D79">
         <v>5700</v>
       </c>
-    </row>
-    <row r="80" spans="1:4" x14ac:dyDescent="0.25">
+      <c r="E79">
+        <v>5871</v>
+      </c>
+    </row>
+    <row r="80" spans="1:5" x14ac:dyDescent="0.25">
       <c r="A80">
         <v>72</v>
       </c>
@@ -4710,8 +5299,11 @@
       <c r="D80">
         <v>5700</v>
       </c>
-    </row>
-    <row r="81" spans="1:4" x14ac:dyDescent="0.25">
+      <c r="E80">
+        <v>5871</v>
+      </c>
+    </row>
+    <row r="81" spans="1:5" x14ac:dyDescent="0.25">
       <c r="A81">
         <v>73</v>
       </c>
@@ -4721,8 +5313,11 @@
       <c r="D81">
         <v>5472</v>
       </c>
-    </row>
-    <row r="82" spans="1:4" x14ac:dyDescent="0.25">
+      <c r="E81">
+        <v>6180</v>
+      </c>
+    </row>
+    <row r="82" spans="1:5" x14ac:dyDescent="0.25">
       <c r="A82">
         <v>74</v>
       </c>
@@ -4732,8 +5327,11 @@
       <c r="D82">
         <v>5643</v>
       </c>
-    </row>
-    <row r="83" spans="1:4" x14ac:dyDescent="0.25">
+      <c r="E82">
+        <v>5871</v>
+      </c>
+    </row>
+    <row r="83" spans="1:5" x14ac:dyDescent="0.25">
       <c r="A83">
         <v>75</v>
       </c>
@@ -4743,8 +5341,11 @@
       <c r="D83">
         <v>5700</v>
       </c>
-    </row>
-    <row r="84" spans="1:4" x14ac:dyDescent="0.25">
+      <c r="E83">
+        <v>6180</v>
+      </c>
+    </row>
+    <row r="84" spans="1:5" x14ac:dyDescent="0.25">
       <c r="A84">
         <v>76</v>
       </c>
@@ -4754,8 +5355,11 @@
       <c r="D84">
         <v>5700</v>
       </c>
-    </row>
-    <row r="85" spans="1:4" x14ac:dyDescent="0.25">
+      <c r="E84">
+        <v>5871</v>
+      </c>
+    </row>
+    <row r="85" spans="1:5" x14ac:dyDescent="0.25">
       <c r="A85">
         <v>77</v>
       </c>
@@ -4765,8 +5369,11 @@
       <c r="D85">
         <v>5700</v>
       </c>
-    </row>
-    <row r="86" spans="1:4" x14ac:dyDescent="0.25">
+      <c r="E85">
+        <v>5871</v>
+      </c>
+    </row>
+    <row r="86" spans="1:5" x14ac:dyDescent="0.25">
       <c r="A86">
         <v>78</v>
       </c>
@@ -4776,8 +5383,11 @@
       <c r="D86">
         <v>5700</v>
       </c>
-    </row>
-    <row r="87" spans="1:4" x14ac:dyDescent="0.25">
+      <c r="E86">
+        <v>6180</v>
+      </c>
+    </row>
+    <row r="87" spans="1:5" x14ac:dyDescent="0.25">
       <c r="A87">
         <v>79</v>
       </c>
@@ -4787,8 +5397,11 @@
       <c r="D87">
         <v>5643</v>
       </c>
-    </row>
-    <row r="88" spans="1:4" x14ac:dyDescent="0.25">
+      <c r="E87">
+        <v>5871</v>
+      </c>
+    </row>
+    <row r="88" spans="1:5" x14ac:dyDescent="0.25">
       <c r="A88">
         <v>80</v>
       </c>
@@ -4798,8 +5411,11 @@
       <c r="D88">
         <v>5529</v>
       </c>
-    </row>
-    <row r="89" spans="1:4" x14ac:dyDescent="0.25">
+      <c r="E88">
+        <v>6180</v>
+      </c>
+    </row>
+    <row r="89" spans="1:5" x14ac:dyDescent="0.25">
       <c r="A89">
         <v>81</v>
       </c>
@@ -4809,8 +5425,11 @@
       <c r="D89">
         <v>5643</v>
       </c>
-    </row>
-    <row r="90" spans="1:4" x14ac:dyDescent="0.25">
+      <c r="E89">
+        <v>5871</v>
+      </c>
+    </row>
+    <row r="90" spans="1:5" x14ac:dyDescent="0.25">
       <c r="A90">
         <v>82</v>
       </c>
@@ -4820,8 +5439,11 @@
       <c r="D90">
         <v>5700</v>
       </c>
-    </row>
-    <row r="91" spans="1:4" x14ac:dyDescent="0.25">
+      <c r="E90">
+        <v>5871</v>
+      </c>
+    </row>
+    <row r="91" spans="1:5" x14ac:dyDescent="0.25">
       <c r="A91">
         <v>83</v>
       </c>
@@ -4831,8 +5453,11 @@
       <c r="D91">
         <v>5700</v>
       </c>
-    </row>
-    <row r="92" spans="1:4" x14ac:dyDescent="0.25">
+      <c r="E91">
+        <v>6180</v>
+      </c>
+    </row>
+    <row r="92" spans="1:5" x14ac:dyDescent="0.25">
       <c r="A92">
         <v>84</v>
       </c>
@@ -4842,8 +5467,11 @@
       <c r="D92">
         <v>5700</v>
       </c>
-    </row>
-    <row r="93" spans="1:4" x14ac:dyDescent="0.25">
+      <c r="E92">
+        <v>5871</v>
+      </c>
+    </row>
+    <row r="93" spans="1:5" x14ac:dyDescent="0.25">
       <c r="A93">
         <v>85</v>
       </c>
@@ -4853,8 +5481,11 @@
       <c r="D93">
         <v>5700</v>
       </c>
-    </row>
-    <row r="94" spans="1:4" x14ac:dyDescent="0.25">
+      <c r="E93">
+        <v>6180</v>
+      </c>
+    </row>
+    <row r="94" spans="1:5" x14ac:dyDescent="0.25">
       <c r="A94">
         <v>86</v>
       </c>
@@ -4864,8 +5495,11 @@
       <c r="D94">
         <v>5643</v>
       </c>
-    </row>
-    <row r="95" spans="1:4" x14ac:dyDescent="0.25">
+      <c r="E94">
+        <v>5871</v>
+      </c>
+    </row>
+    <row r="95" spans="1:5" x14ac:dyDescent="0.25">
       <c r="A95">
         <v>87</v>
       </c>
@@ -4875,8 +5509,11 @@
       <c r="D95">
         <v>5529</v>
       </c>
-    </row>
-    <row r="96" spans="1:4" x14ac:dyDescent="0.25">
+      <c r="E95">
+        <v>5871</v>
+      </c>
+    </row>
+    <row r="96" spans="1:5" x14ac:dyDescent="0.25">
       <c r="A96">
         <v>88</v>
       </c>
@@ -4886,8 +5523,11 @@
       <c r="D96">
         <v>5643</v>
       </c>
-    </row>
-    <row r="97" spans="1:4" x14ac:dyDescent="0.25">
+      <c r="E96">
+        <v>6180</v>
+      </c>
+    </row>
+    <row r="97" spans="1:5" x14ac:dyDescent="0.25">
       <c r="A97">
         <v>89</v>
       </c>
@@ -4897,8 +5537,11 @@
       <c r="D97">
         <v>5700</v>
       </c>
-    </row>
-    <row r="98" spans="1:4" x14ac:dyDescent="0.25">
+      <c r="E97">
+        <v>5871</v>
+      </c>
+    </row>
+    <row r="98" spans="1:5" x14ac:dyDescent="0.25">
       <c r="A98">
         <v>90</v>
       </c>
@@ -4908,8 +5551,11 @@
       <c r="D98">
         <v>5700</v>
       </c>
-    </row>
-    <row r="99" spans="1:4" x14ac:dyDescent="0.25">
+      <c r="E98">
+        <v>5871</v>
+      </c>
+    </row>
+    <row r="99" spans="1:5" x14ac:dyDescent="0.25">
       <c r="A99">
         <v>91</v>
       </c>
@@ -4919,8 +5565,11 @@
       <c r="D99">
         <v>5700</v>
       </c>
-    </row>
-    <row r="100" spans="1:4" x14ac:dyDescent="0.25">
+      <c r="E99">
+        <v>6180</v>
+      </c>
+    </row>
+    <row r="100" spans="1:5" x14ac:dyDescent="0.25">
       <c r="A100">
         <v>92</v>
       </c>
@@ -4930,8 +5579,11 @@
       <c r="D100">
         <v>5586</v>
       </c>
-    </row>
-    <row r="101" spans="1:4" x14ac:dyDescent="0.25">
+      <c r="E100">
+        <v>5871</v>
+      </c>
+    </row>
+    <row r="101" spans="1:5" x14ac:dyDescent="0.25">
       <c r="A101">
         <v>93</v>
       </c>
@@ -4941,8 +5593,11 @@
       <c r="D101">
         <v>5529</v>
       </c>
-    </row>
-    <row r="102" spans="1:4" x14ac:dyDescent="0.25">
+      <c r="E101">
+        <v>6180</v>
+      </c>
+    </row>
+    <row r="102" spans="1:5" x14ac:dyDescent="0.25">
       <c r="A102">
         <v>94</v>
       </c>
@@ -4952,8 +5607,11 @@
       <c r="D102">
         <v>5700</v>
       </c>
-    </row>
-    <row r="103" spans="1:4" x14ac:dyDescent="0.25">
+      <c r="E102">
+        <v>5871</v>
+      </c>
+    </row>
+    <row r="103" spans="1:5" x14ac:dyDescent="0.25">
       <c r="A103">
         <v>95</v>
       </c>
@@ -4963,8 +5621,11 @@
       <c r="D103">
         <v>5700</v>
       </c>
-    </row>
-    <row r="104" spans="1:4" x14ac:dyDescent="0.25">
+      <c r="E103">
+        <v>5871</v>
+      </c>
+    </row>
+    <row r="104" spans="1:5" x14ac:dyDescent="0.25">
       <c r="A104">
         <v>96</v>
       </c>
@@ -4974,8 +5635,11 @@
       <c r="D104">
         <v>5700</v>
       </c>
-    </row>
-    <row r="105" spans="1:4" x14ac:dyDescent="0.25">
+      <c r="E104">
+        <v>6180</v>
+      </c>
+    </row>
+    <row r="105" spans="1:5" x14ac:dyDescent="0.25">
       <c r="A105">
         <v>97</v>
       </c>
@@ -4985,8 +5649,11 @@
       <c r="D105">
         <v>5700</v>
       </c>
-    </row>
-    <row r="106" spans="1:4" x14ac:dyDescent="0.25">
+      <c r="E105">
+        <v>5871</v>
+      </c>
+    </row>
+    <row r="106" spans="1:5" x14ac:dyDescent="0.25">
       <c r="A106">
         <v>98</v>
       </c>
@@ -4996,8 +5663,11 @@
       <c r="D106">
         <v>5700</v>
       </c>
-    </row>
-    <row r="107" spans="1:4" x14ac:dyDescent="0.25">
+      <c r="E106">
+        <v>6180</v>
+      </c>
+    </row>
+    <row r="107" spans="1:5" x14ac:dyDescent="0.25">
       <c r="A107">
         <v>99</v>
       </c>
@@ -5007,8 +5677,11 @@
       <c r="D107">
         <v>5586</v>
       </c>
-    </row>
-    <row r="108" spans="1:4" x14ac:dyDescent="0.25">
+      <c r="E107">
+        <v>5871</v>
+      </c>
+    </row>
+    <row r="108" spans="1:5" x14ac:dyDescent="0.25">
       <c r="A108">
         <v>100</v>
       </c>
@@ -5018,8 +5691,11 @@
       <c r="D108">
         <v>5586</v>
       </c>
-    </row>
-    <row r="109" spans="1:4" x14ac:dyDescent="0.25">
+      <c r="E108">
+        <v>6180</v>
+      </c>
+    </row>
+    <row r="109" spans="1:5" x14ac:dyDescent="0.25">
       <c r="A109">
         <v>101</v>
       </c>
@@ -5029,8 +5705,11 @@
       <c r="D109">
         <v>5643</v>
       </c>
-    </row>
-    <row r="110" spans="1:4" x14ac:dyDescent="0.25">
+      <c r="E109">
+        <v>5871</v>
+      </c>
+    </row>
+    <row r="110" spans="1:5" x14ac:dyDescent="0.25">
       <c r="A110">
         <v>102</v>
       </c>
@@ -5040,8 +5719,11 @@
       <c r="D110">
         <v>5700</v>
       </c>
-    </row>
-    <row r="111" spans="1:4" x14ac:dyDescent="0.25">
+      <c r="E110">
+        <v>6180</v>
+      </c>
+    </row>
+    <row r="111" spans="1:5" x14ac:dyDescent="0.25">
       <c r="A111">
         <v>103</v>
       </c>
@@ -5052,7 +5734,7 @@
         <v>5700</v>
       </c>
     </row>
-    <row r="112" spans="1:4" x14ac:dyDescent="0.25">
+    <row r="112" spans="1:5" x14ac:dyDescent="0.25">
       <c r="A112">
         <v>104</v>
       </c>
@@ -5364,6 +6046,9 @@
       </c>
     </row>
   </sheetData>
+  <mergeCells count="1">
+    <mergeCell ref="B1:E1"/>
+  </mergeCells>
   <pageMargins left="0.7" right="0.7" top="0.75" bottom="0.75" header="0.3" footer="0.3"/>
   <drawing r:id="rId1"/>
 </worksheet>
@@ -5371,18 +6056,29 @@
 
 <file path=xl/worksheets/sheet2.xml><?xml version="1.0" encoding="utf-8"?>
 <worksheet xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" xmlns:r="http://schemas.openxmlformats.org/officeDocument/2006/relationships" xmlns:mc="http://schemas.openxmlformats.org/markup-compatibility/2006" xmlns:x14ac="http://schemas.microsoft.com/office/spreadsheetml/2009/9/ac" xmlns:xr="http://schemas.microsoft.com/office/spreadsheetml/2014/revision" xmlns:xr2="http://schemas.microsoft.com/office/spreadsheetml/2015/revision2" xmlns:xr3="http://schemas.microsoft.com/office/spreadsheetml/2016/revision3" mc:Ignorable="x14ac xr xr2 xr3" xr:uid="{FA2434C9-9FEE-4B74-A6E8-22FF2ED6C4F5}">
-  <dimension ref="A2:D149"/>
+  <dimension ref="A1:D149"/>
   <sheetViews>
-    <sheetView tabSelected="1" topLeftCell="A13" workbookViewId="0">
-      <selection activeCell="H37" sqref="H37"/>
+    <sheetView workbookViewId="0">
+      <selection activeCell="F4" sqref="F4"/>
     </sheetView>
   </sheetViews>
   <sheetFormatPr defaultRowHeight="15" x14ac:dyDescent="0.25"/>
   <cols>
-    <col min="2" max="2" width="5" bestFit="1" customWidth="1"/>
+    <col min="2" max="2" width="7" bestFit="1" customWidth="1"/>
     <col min="3" max="3" width="11.7109375" bestFit="1" customWidth="1"/>
+    <col min="4" max="4" width="5.85546875" bestFit="1" customWidth="1"/>
   </cols>
   <sheetData>
+    <row r="1" spans="1:4" x14ac:dyDescent="0.25">
+      <c r="A1" t="s">
+        <v>0</v>
+      </c>
+      <c r="B1" s="1" t="s">
+        <v>8</v>
+      </c>
+      <c r="C1" s="1"/>
+      <c r="D1" s="1"/>
+    </row>
     <row r="2" spans="1:4" x14ac:dyDescent="0.25">
       <c r="B2" t="s">
         <v>5</v>
@@ -5428,11 +6124,31 @@
       <c r="A9">
         <v>-4</v>
       </c>
+      <c r="B9">
+        <v>0</v>
+      </c>
+      <c r="C9">
+        <v>281</v>
+      </c>
+      <c r="D9">
+        <f>C9-C8</f>
+        <v>281</v>
+      </c>
     </row>
     <row r="10" spans="1:4" x14ac:dyDescent="0.25">
       <c r="A10">
         <v>-3</v>
       </c>
+      <c r="B10">
+        <v>0</v>
+      </c>
+      <c r="C10">
+        <v>414</v>
+      </c>
+      <c r="D10">
+        <f>C10-C9</f>
+        <v>133</v>
+      </c>
     </row>
     <row r="11" spans="1:4" x14ac:dyDescent="0.25">
       <c r="A11">
@@ -5442,11 +6158,11 @@
         <v>0</v>
       </c>
       <c r="C11">
-        <v>131</v>
+        <v>469</v>
       </c>
       <c r="D11">
         <f>C11-C10</f>
-        <v>131</v>
+        <v>55</v>
       </c>
     </row>
     <row r="12" spans="1:4" x14ac:dyDescent="0.25">
@@ -5457,11 +6173,11 @@
         <v>0</v>
       </c>
       <c r="C12">
-        <v>392</v>
+        <v>575</v>
       </c>
       <c r="D12">
         <f t="shared" ref="D12:D75" si="0">C12-C11</f>
-        <v>261</v>
+        <v>106</v>
       </c>
     </row>
     <row r="13" spans="1:4" x14ac:dyDescent="0.25">
@@ -5472,11 +6188,11 @@
         <v>0</v>
       </c>
       <c r="C13">
-        <v>684</v>
+        <v>839</v>
       </c>
       <c r="D13">
         <f t="shared" si="0"/>
-        <v>292</v>
+        <v>264</v>
       </c>
     </row>
     <row r="14" spans="1:4" x14ac:dyDescent="0.25">
@@ -5484,14 +6200,14 @@
         <v>1</v>
       </c>
       <c r="B14">
-        <v>391</v>
+        <v>308</v>
       </c>
       <c r="C14">
-        <v>967</v>
+        <v>1121</v>
       </c>
       <c r="D14">
         <f t="shared" si="0"/>
-        <v>283</v>
+        <v>282</v>
       </c>
     </row>
     <row r="15" spans="1:4" x14ac:dyDescent="0.25">
@@ -5499,10 +6215,10 @@
         <v>2</v>
       </c>
       <c r="B15">
-        <v>0</v>
+        <v>83</v>
       </c>
       <c r="C15">
-        <v>1259</v>
+        <v>1413</v>
       </c>
       <c r="D15">
         <f t="shared" si="0"/>
@@ -5514,14 +6230,14 @@
         <v>3</v>
       </c>
       <c r="B16">
-        <v>0</v>
+        <v>539</v>
       </c>
       <c r="C16">
-        <v>1552</v>
+        <v>1705</v>
       </c>
       <c r="D16">
         <f t="shared" si="0"/>
-        <v>293</v>
+        <v>292</v>
       </c>
     </row>
     <row r="17" spans="1:4" x14ac:dyDescent="0.25">
@@ -5529,14 +6245,14 @@
         <v>4</v>
       </c>
       <c r="B17">
-        <v>0</v>
+        <v>1268</v>
       </c>
       <c r="C17">
-        <v>1845</v>
+        <v>1997</v>
       </c>
       <c r="D17">
         <f t="shared" si="0"/>
-        <v>293</v>
+        <v>292</v>
       </c>
     </row>
     <row r="18" spans="1:4" x14ac:dyDescent="0.25">
@@ -5544,14 +6260,14 @@
         <v>5</v>
       </c>
       <c r="B18">
-        <v>0</v>
+        <v>1825</v>
       </c>
       <c r="C18">
-        <v>2136</v>
+        <v>2290</v>
       </c>
       <c r="D18">
         <f t="shared" si="0"/>
-        <v>291</v>
+        <v>293</v>
       </c>
     </row>
     <row r="19" spans="1:4" x14ac:dyDescent="0.25">
@@ -5559,14 +6275,14 @@
         <v>6</v>
       </c>
       <c r="B19">
-        <v>0</v>
+        <v>2588</v>
       </c>
       <c r="C19">
-        <v>2430</v>
+        <v>2582</v>
       </c>
       <c r="D19">
         <f t="shared" si="0"/>
-        <v>294</v>
+        <v>292</v>
       </c>
     </row>
     <row r="20" spans="1:4" x14ac:dyDescent="0.25">
@@ -5574,14 +6290,14 @@
         <v>7</v>
       </c>
       <c r="B20">
-        <v>0</v>
+        <v>3079</v>
       </c>
       <c r="C20">
-        <v>2724</v>
+        <v>2874</v>
       </c>
       <c r="D20">
         <f t="shared" si="0"/>
-        <v>294</v>
+        <v>292</v>
       </c>
     </row>
     <row r="21" spans="1:4" x14ac:dyDescent="0.25">
@@ -5589,10 +6305,10 @@
         <v>8</v>
       </c>
       <c r="B21">
-        <v>0</v>
+        <v>3706</v>
       </c>
       <c r="C21">
-        <v>3016</v>
+        <v>3166</v>
       </c>
       <c r="D21">
         <f t="shared" si="0"/>
@@ -5604,14 +6320,14 @@
         <v>9</v>
       </c>
       <c r="B22">
-        <v>0</v>
+        <v>4711</v>
       </c>
       <c r="C22">
-        <v>3309</v>
+        <v>3458</v>
       </c>
       <c r="D22">
         <f t="shared" si="0"/>
-        <v>293</v>
+        <v>292</v>
       </c>
     </row>
     <row r="23" spans="1:4" x14ac:dyDescent="0.25">
@@ -5619,10 +6335,10 @@
         <v>10</v>
       </c>
       <c r="B23">
-        <v>70</v>
+        <v>5440</v>
       </c>
       <c r="C23">
-        <v>3602</v>
+        <v>3751</v>
       </c>
       <c r="D23">
         <f t="shared" si="0"/>
@@ -5634,14 +6350,14 @@
         <v>11</v>
       </c>
       <c r="B24">
-        <v>132</v>
+        <v>6687</v>
       </c>
       <c r="C24">
-        <v>3894</v>
+        <v>4045</v>
       </c>
       <c r="D24">
         <f t="shared" si="0"/>
-        <v>292</v>
+        <v>294</v>
       </c>
     </row>
     <row r="25" spans="1:4" x14ac:dyDescent="0.25">
@@ -5649,14 +6365,14 @@
         <v>12</v>
       </c>
       <c r="B25">
-        <v>132</v>
+        <v>7700</v>
       </c>
       <c r="C25">
-        <v>4187</v>
+        <v>4337</v>
       </c>
       <c r="D25">
         <f t="shared" si="0"/>
-        <v>293</v>
+        <v>292</v>
       </c>
     </row>
     <row r="26" spans="1:4" x14ac:dyDescent="0.25">
@@ -5664,14 +6380,14 @@
         <v>13</v>
       </c>
       <c r="B26">
-        <v>132</v>
+        <v>8233</v>
       </c>
       <c r="C26">
-        <v>4481</v>
+        <v>4630</v>
       </c>
       <c r="D26">
         <f t="shared" si="0"/>
-        <v>294</v>
+        <v>293</v>
       </c>
     </row>
     <row r="27" spans="1:4" x14ac:dyDescent="0.25">
@@ -5679,14 +6395,14 @@
         <v>14</v>
       </c>
       <c r="B27">
-        <v>132</v>
+        <v>9660</v>
       </c>
       <c r="C27">
-        <v>4774</v>
+        <v>4922</v>
       </c>
       <c r="D27">
         <f t="shared" si="0"/>
-        <v>293</v>
+        <v>292</v>
       </c>
     </row>
     <row r="28" spans="1:4" x14ac:dyDescent="0.25">
@@ -5694,14 +6410,14 @@
         <v>15</v>
       </c>
       <c r="B28">
-        <v>132</v>
+        <v>10239</v>
       </c>
       <c r="C28">
-        <v>5067</v>
+        <v>5214</v>
       </c>
       <c r="D28">
         <f t="shared" si="0"/>
-        <v>293</v>
+        <v>292</v>
       </c>
     </row>
     <row r="29" spans="1:4" x14ac:dyDescent="0.25">
@@ -5709,14 +6425,14 @@
         <v>16</v>
       </c>
       <c r="B29">
-        <v>132</v>
+        <v>11386</v>
       </c>
       <c r="C29">
-        <v>5362</v>
+        <v>5506</v>
       </c>
       <c r="D29">
         <f t="shared" si="0"/>
-        <v>295</v>
+        <v>292</v>
       </c>
     </row>
     <row r="30" spans="1:4" x14ac:dyDescent="0.25">
@@ -5724,10 +6440,10 @@
         <v>17</v>
       </c>
       <c r="B30">
-        <v>132</v>
+        <v>13224</v>
       </c>
       <c r="C30">
-        <v>5655</v>
+        <v>5799</v>
       </c>
       <c r="D30">
         <f t="shared" si="0"/>
@@ -5739,14 +6455,14 @@
         <v>18</v>
       </c>
       <c r="B31">
-        <v>132</v>
+        <v>14444</v>
       </c>
       <c r="C31">
-        <v>5949</v>
+        <v>6092</v>
       </c>
       <c r="D31">
         <f t="shared" si="0"/>
-        <v>294</v>
+        <v>293</v>
       </c>
     </row>
     <row r="32" spans="1:4" x14ac:dyDescent="0.25">
@@ -5754,14 +6470,14 @@
         <v>19</v>
       </c>
       <c r="B32">
-        <v>132</v>
+        <v>14924</v>
       </c>
       <c r="C32">
-        <v>6244</v>
+        <v>6386</v>
       </c>
       <c r="D32">
         <f t="shared" si="0"/>
-        <v>295</v>
+        <v>294</v>
       </c>
     </row>
     <row r="33" spans="1:4" x14ac:dyDescent="0.25">
@@ -5769,14 +6485,14 @@
         <v>20</v>
       </c>
       <c r="B33">
-        <v>132</v>
+        <v>16884</v>
       </c>
       <c r="C33">
-        <v>6536</v>
+        <v>6679</v>
       </c>
       <c r="D33">
         <f t="shared" si="0"/>
-        <v>292</v>
+        <v>293</v>
       </c>
     </row>
     <row r="34" spans="1:4" x14ac:dyDescent="0.25">
@@ -5784,14 +6500,14 @@
         <v>21</v>
       </c>
       <c r="B34">
-        <v>128</v>
+        <v>17181</v>
       </c>
       <c r="C34">
-        <v>6829</v>
+        <v>6971</v>
       </c>
       <c r="D34">
         <f t="shared" si="0"/>
-        <v>293</v>
+        <v>292</v>
       </c>
     </row>
     <row r="35" spans="1:4" x14ac:dyDescent="0.25">
@@ -5799,10 +6515,10 @@
         <v>22</v>
       </c>
       <c r="B35">
-        <v>132</v>
+        <v>19324</v>
       </c>
       <c r="C35">
-        <v>7122</v>
+        <v>7264</v>
       </c>
       <c r="D35">
         <f t="shared" si="0"/>
@@ -5814,14 +6530,14 @@
         <v>23</v>
       </c>
       <c r="B36">
-        <v>132</v>
+        <v>19511</v>
       </c>
       <c r="C36">
-        <v>7414</v>
+        <v>7557</v>
       </c>
       <c r="D36">
         <f t="shared" si="0"/>
-        <v>292</v>
+        <v>293</v>
       </c>
     </row>
     <row r="37" spans="1:4" x14ac:dyDescent="0.25">
@@ -5829,14 +6545,14 @@
         <v>24</v>
       </c>
       <c r="B37">
-        <v>132</v>
+        <v>21764</v>
       </c>
       <c r="C37">
-        <v>7705</v>
+        <v>7850</v>
       </c>
       <c r="D37">
         <f t="shared" si="0"/>
-        <v>291</v>
+        <v>293</v>
       </c>
     </row>
     <row r="38" spans="1:4" x14ac:dyDescent="0.25">
@@ -5844,14 +6560,14 @@
         <v>25</v>
       </c>
       <c r="B38">
-        <v>132</v>
+        <v>21845</v>
       </c>
       <c r="C38">
-        <v>7997</v>
+        <v>8141</v>
       </c>
       <c r="D38">
         <f t="shared" si="0"/>
-        <v>292</v>
+        <v>291</v>
       </c>
     </row>
     <row r="39" spans="1:4" x14ac:dyDescent="0.25">
@@ -5859,10 +6575,10 @@
         <v>26</v>
       </c>
       <c r="B39">
-        <v>132</v>
+        <v>24204</v>
       </c>
       <c r="C39">
-        <v>8289</v>
+        <v>8433</v>
       </c>
       <c r="D39">
         <f t="shared" si="0"/>
@@ -5874,14 +6590,14 @@
         <v>27</v>
       </c>
       <c r="B40">
-        <v>132</v>
+        <v>24196</v>
       </c>
       <c r="C40">
-        <v>8581</v>
+        <v>8726</v>
       </c>
       <c r="D40">
         <f t="shared" si="0"/>
-        <v>292</v>
+        <v>293</v>
       </c>
     </row>
     <row r="41" spans="1:4" x14ac:dyDescent="0.25">
@@ -5889,14 +6605,14 @@
         <v>28</v>
       </c>
       <c r="B41">
-        <v>132</v>
+        <v>26644</v>
       </c>
       <c r="C41">
-        <v>8873</v>
+        <v>9019</v>
       </c>
       <c r="D41">
         <f t="shared" si="0"/>
-        <v>292</v>
+        <v>293</v>
       </c>
     </row>
     <row r="42" spans="1:4" x14ac:dyDescent="0.25">
@@ -5904,10 +6620,10 @@
         <v>29</v>
       </c>
       <c r="B42">
-        <v>132</v>
+        <v>26453</v>
       </c>
       <c r="C42">
-        <v>9165</v>
+        <v>9311</v>
       </c>
       <c r="D42">
         <f t="shared" si="0"/>
@@ -5919,14 +6635,14 @@
         <v>30</v>
       </c>
       <c r="B43">
-        <v>132</v>
+        <v>29084</v>
       </c>
       <c r="C43">
-        <v>9457</v>
+        <v>9605</v>
       </c>
       <c r="D43">
         <f t="shared" si="0"/>
-        <v>292</v>
+        <v>294</v>
       </c>
     </row>
     <row r="44" spans="1:4" x14ac:dyDescent="0.25">
@@ -5934,10 +6650,10 @@
         <v>31</v>
       </c>
       <c r="B44">
-        <v>132</v>
+        <v>28771</v>
       </c>
       <c r="C44">
-        <v>9749</v>
+        <v>9897</v>
       </c>
       <c r="D44">
         <f t="shared" si="0"/>
@@ -5949,10 +6665,10 @@
         <v>32</v>
       </c>
       <c r="B45">
-        <v>132</v>
+        <v>31524</v>
       </c>
       <c r="C45">
-        <v>10041</v>
+        <v>10189</v>
       </c>
       <c r="D45">
         <f t="shared" si="0"/>
@@ -5964,10 +6680,10 @@
         <v>33</v>
       </c>
       <c r="B46">
-        <v>132</v>
+        <v>31101</v>
       </c>
       <c r="C46">
-        <v>10332</v>
+        <v>10480</v>
       </c>
       <c r="D46">
         <f t="shared" si="0"/>
@@ -5979,10 +6695,10 @@
         <v>34</v>
       </c>
       <c r="B47">
-        <v>132</v>
+        <v>33964</v>
       </c>
       <c r="C47">
-        <v>10625</v>
+        <v>10773</v>
       </c>
       <c r="D47">
         <f t="shared" si="0"/>
@@ -5994,14 +6710,14 @@
         <v>35</v>
       </c>
       <c r="B48">
-        <v>132</v>
+        <v>33407</v>
       </c>
       <c r="C48">
-        <v>10916</v>
+        <v>11066</v>
       </c>
       <c r="D48">
         <f t="shared" si="0"/>
-        <v>291</v>
+        <v>293</v>
       </c>
     </row>
     <row r="49" spans="1:4" x14ac:dyDescent="0.25">
@@ -6009,10 +6725,10 @@
         <v>36</v>
       </c>
       <c r="B49">
-        <v>132</v>
+        <v>36404</v>
       </c>
       <c r="C49">
-        <v>11209</v>
+        <v>11359</v>
       </c>
       <c r="D49">
         <f t="shared" si="0"/>
@@ -6024,14 +6740,14 @@
         <v>37</v>
       </c>
       <c r="B50">
-        <v>132</v>
+        <v>35725</v>
       </c>
       <c r="C50">
-        <v>11500</v>
+        <v>11652</v>
       </c>
       <c r="D50">
         <f t="shared" si="0"/>
-        <v>291</v>
+        <v>293</v>
       </c>
     </row>
     <row r="51" spans="1:4" x14ac:dyDescent="0.25">
@@ -6039,14 +6755,14 @@
         <v>38</v>
       </c>
       <c r="B51">
-        <v>132</v>
+        <v>38844</v>
       </c>
       <c r="C51">
-        <v>11792</v>
+        <v>11945</v>
       </c>
       <c r="D51">
         <f t="shared" si="0"/>
-        <v>292</v>
+        <v>293</v>
       </c>
     </row>
     <row r="52" spans="1:4" x14ac:dyDescent="0.25">
@@ -6054,14 +6770,14 @@
         <v>39</v>
       </c>
       <c r="B52">
-        <v>132</v>
+        <v>38043</v>
       </c>
       <c r="C52">
-        <v>12083</v>
+        <v>12238</v>
       </c>
       <c r="D52">
         <f t="shared" si="0"/>
-        <v>291</v>
+        <v>293</v>
       </c>
     </row>
     <row r="53" spans="1:4" x14ac:dyDescent="0.25">
@@ -6069,14 +6785,14 @@
         <v>40</v>
       </c>
       <c r="B53">
-        <v>136</v>
+        <v>41284</v>
       </c>
       <c r="C53">
-        <v>12375</v>
+        <v>12531</v>
       </c>
       <c r="D53">
         <f t="shared" si="0"/>
-        <v>292</v>
+        <v>293</v>
       </c>
     </row>
     <row r="54" spans="1:4" x14ac:dyDescent="0.25">
@@ -6084,10 +6800,10 @@
         <v>41</v>
       </c>
       <c r="B54">
-        <v>132</v>
+        <v>40361</v>
       </c>
       <c r="C54">
-        <v>12667</v>
+        <v>12823</v>
       </c>
       <c r="D54">
         <f t="shared" si="0"/>
@@ -6099,14 +6815,14 @@
         <v>42</v>
       </c>
       <c r="B55">
-        <v>132</v>
+        <v>43724</v>
       </c>
       <c r="C55">
-        <v>12957</v>
+        <v>13114</v>
       </c>
       <c r="D55">
         <f t="shared" si="0"/>
-        <v>290</v>
+        <v>291</v>
       </c>
     </row>
     <row r="56" spans="1:4" x14ac:dyDescent="0.25">
@@ -6114,14 +6830,14 @@
         <v>43</v>
       </c>
       <c r="B56">
-        <v>132</v>
+        <v>42679</v>
       </c>
       <c r="C56">
-        <v>13248</v>
+        <v>13406</v>
       </c>
       <c r="D56">
         <f t="shared" si="0"/>
-        <v>291</v>
+        <v>292</v>
       </c>
     </row>
     <row r="57" spans="1:4" x14ac:dyDescent="0.25">
@@ -6129,14 +6845,14 @@
         <v>44</v>
       </c>
       <c r="B57">
-        <v>132</v>
+        <v>46164</v>
       </c>
       <c r="C57">
-        <v>13541</v>
+        <v>13698</v>
       </c>
       <c r="D57">
         <f t="shared" si="0"/>
-        <v>293</v>
+        <v>292</v>
       </c>
     </row>
     <row r="58" spans="1:4" x14ac:dyDescent="0.25">
@@ -6144,14 +6860,14 @@
         <v>45</v>
       </c>
       <c r="B58">
-        <v>132</v>
+        <v>45009</v>
       </c>
       <c r="C58">
-        <v>13832</v>
+        <v>13991</v>
       </c>
       <c r="D58">
         <f t="shared" si="0"/>
-        <v>291</v>
+        <v>293</v>
       </c>
     </row>
     <row r="59" spans="1:4" x14ac:dyDescent="0.25">
@@ -6159,14 +6875,14 @@
         <v>46</v>
       </c>
       <c r="B59">
-        <v>132</v>
+        <v>48604</v>
       </c>
       <c r="C59">
-        <v>14124</v>
+        <v>14284</v>
       </c>
       <c r="D59">
         <f t="shared" si="0"/>
-        <v>292</v>
+        <v>293</v>
       </c>
     </row>
     <row r="60" spans="1:4" x14ac:dyDescent="0.25">
@@ -6174,14 +6890,14 @@
         <v>47</v>
       </c>
       <c r="B60">
-        <v>132</v>
+        <v>47315</v>
       </c>
       <c r="C60">
-        <v>14415</v>
+        <v>14577</v>
       </c>
       <c r="D60">
         <f t="shared" si="0"/>
-        <v>291</v>
+        <v>293</v>
       </c>
     </row>
     <row r="61" spans="1:4" x14ac:dyDescent="0.25">
@@ -6189,14 +6905,14 @@
         <v>48</v>
       </c>
       <c r="B61">
-        <v>132</v>
+        <v>51044</v>
       </c>
       <c r="C61">
-        <v>14707</v>
+        <v>14871</v>
       </c>
       <c r="D61">
         <f t="shared" si="0"/>
-        <v>292</v>
+        <v>294</v>
       </c>
     </row>
     <row r="62" spans="1:4" x14ac:dyDescent="0.25">
@@ -6204,14 +6920,14 @@
         <v>49</v>
       </c>
       <c r="B62">
-        <v>161</v>
+        <v>49633</v>
       </c>
       <c r="C62">
-        <v>14998</v>
+        <v>15163</v>
       </c>
       <c r="D62">
         <f t="shared" si="0"/>
-        <v>291</v>
+        <v>292</v>
       </c>
     </row>
     <row r="63" spans="1:4" x14ac:dyDescent="0.25">
@@ -6219,14 +6935,14 @@
         <v>50</v>
       </c>
       <c r="B63">
-        <v>103</v>
+        <v>53484</v>
       </c>
       <c r="C63">
-        <v>15289</v>
+        <v>15455</v>
       </c>
       <c r="D63">
         <f t="shared" si="0"/>
-        <v>291</v>
+        <v>292</v>
       </c>
     </row>
     <row r="64" spans="1:4" x14ac:dyDescent="0.25">
@@ -6234,10 +6950,10 @@
         <v>51</v>
       </c>
       <c r="B64">
-        <v>132</v>
+        <v>51951</v>
       </c>
       <c r="C64">
-        <v>15580</v>
+        <v>15746</v>
       </c>
       <c r="D64">
         <f t="shared" si="0"/>
@@ -6249,14 +6965,14 @@
         <v>52</v>
       </c>
       <c r="B65">
-        <v>132</v>
+        <v>55924</v>
       </c>
       <c r="C65">
-        <v>15872</v>
+        <v>16037</v>
       </c>
       <c r="D65">
         <f t="shared" si="0"/>
-        <v>292</v>
+        <v>291</v>
       </c>
     </row>
     <row r="66" spans="1:4" x14ac:dyDescent="0.25">
@@ -6264,10 +6980,10 @@
         <v>53</v>
       </c>
       <c r="B66">
-        <v>132</v>
+        <v>54281</v>
       </c>
       <c r="C66">
-        <v>16163</v>
+        <v>16328</v>
       </c>
       <c r="D66">
         <f t="shared" si="0"/>
@@ -6279,10 +6995,10 @@
         <v>54</v>
       </c>
       <c r="B67">
-        <v>132</v>
+        <v>55428</v>
       </c>
       <c r="C67">
-        <v>16455</v>
+        <v>16620</v>
       </c>
       <c r="D67">
         <f t="shared" si="0"/>
@@ -6294,14 +7010,14 @@
         <v>55</v>
       </c>
       <c r="B68">
-        <v>132</v>
+        <v>59584</v>
       </c>
       <c r="C68">
-        <v>16746</v>
+        <v>16912</v>
       </c>
       <c r="D68">
         <f t="shared" si="0"/>
-        <v>291</v>
+        <v>292</v>
       </c>
     </row>
     <row r="69" spans="1:4" x14ac:dyDescent="0.25">
@@ -6309,14 +7025,14 @@
         <v>56</v>
       </c>
       <c r="B69">
-        <v>132</v>
+        <v>57746</v>
       </c>
       <c r="C69">
-        <v>17036</v>
+        <v>17205</v>
       </c>
       <c r="D69">
         <f t="shared" si="0"/>
-        <v>290</v>
+        <v>293</v>
       </c>
     </row>
     <row r="70" spans="1:4" x14ac:dyDescent="0.25">
@@ -6324,14 +7040,14 @@
         <v>57</v>
       </c>
       <c r="B70">
-        <v>132</v>
+        <v>61991</v>
       </c>
       <c r="C70">
-        <v>17329</v>
+        <v>17497</v>
       </c>
       <c r="D70">
         <f t="shared" si="0"/>
-        <v>293</v>
+        <v>292</v>
       </c>
     </row>
     <row r="71" spans="1:4" x14ac:dyDescent="0.25">
@@ -6339,10 +7055,10 @@
         <v>58</v>
       </c>
       <c r="B71">
-        <v>132</v>
+        <v>60064</v>
       </c>
       <c r="C71">
-        <v>17621</v>
+        <v>17789</v>
       </c>
       <c r="D71">
         <f t="shared" si="0"/>
@@ -6354,10 +7070,10 @@
         <v>59</v>
       </c>
       <c r="B72">
-        <v>132</v>
+        <v>64464</v>
       </c>
       <c r="C72">
-        <v>17913</v>
+        <v>18081</v>
       </c>
       <c r="D72">
         <f t="shared" si="0"/>
@@ -6369,14 +7085,14 @@
         <v>60</v>
       </c>
       <c r="B73">
-        <v>132</v>
+        <v>62382</v>
       </c>
       <c r="C73">
-        <v>18206</v>
+        <v>18372</v>
       </c>
       <c r="D73">
         <f t="shared" si="0"/>
-        <v>293</v>
+        <v>291</v>
       </c>
     </row>
     <row r="74" spans="1:4" x14ac:dyDescent="0.25">
@@ -6384,14 +7100,14 @@
         <v>61</v>
       </c>
       <c r="B74">
-        <v>132</v>
+        <v>66904</v>
       </c>
       <c r="C74">
-        <v>18498</v>
+        <v>18665</v>
       </c>
       <c r="D74">
         <f t="shared" si="0"/>
-        <v>292</v>
+        <v>293</v>
       </c>
     </row>
     <row r="75" spans="1:4" x14ac:dyDescent="0.25">
@@ -6399,10 +7115,10 @@
         <v>62</v>
       </c>
       <c r="B75">
-        <v>132</v>
+        <v>64700</v>
       </c>
       <c r="C75">
-        <v>18789</v>
+        <v>18956</v>
       </c>
       <c r="D75">
         <f t="shared" si="0"/>
@@ -6414,14 +7130,14 @@
         <v>63</v>
       </c>
       <c r="B76">
-        <v>132</v>
+        <v>69344</v>
       </c>
       <c r="C76">
-        <v>19080</v>
+        <v>19248</v>
       </c>
       <c r="D76">
         <f t="shared" ref="D76:D139" si="1">C76-C75</f>
-        <v>291</v>
+        <v>292</v>
       </c>
     </row>
     <row r="77" spans="1:4" x14ac:dyDescent="0.25">
@@ -6429,10 +7145,10 @@
         <v>64</v>
       </c>
       <c r="B77">
-        <v>132</v>
+        <v>67018</v>
       </c>
       <c r="C77">
-        <v>19372</v>
+        <v>19540</v>
       </c>
       <c r="D77">
         <f t="shared" si="1"/>
@@ -6444,14 +7160,14 @@
         <v>65</v>
       </c>
       <c r="B78">
-        <v>161</v>
+        <v>71784</v>
       </c>
       <c r="C78">
-        <v>19664</v>
+        <v>19834</v>
       </c>
       <c r="D78">
         <f t="shared" si="1"/>
-        <v>292</v>
+        <v>294</v>
       </c>
     </row>
     <row r="79" spans="1:4" x14ac:dyDescent="0.25">
@@ -6459,10 +7175,10 @@
         <v>66</v>
       </c>
       <c r="B79">
-        <v>132</v>
+        <v>69336</v>
       </c>
       <c r="C79">
-        <v>19956</v>
+        <v>20126</v>
       </c>
       <c r="D79">
         <f t="shared" si="1"/>
@@ -6474,14 +7190,14 @@
         <v>67</v>
       </c>
       <c r="B80">
-        <v>136</v>
+        <v>74224</v>
       </c>
       <c r="C80">
-        <v>20248</v>
+        <v>20419</v>
       </c>
       <c r="D80">
         <f t="shared" si="1"/>
-        <v>292</v>
+        <v>293</v>
       </c>
     </row>
     <row r="81" spans="1:4" x14ac:dyDescent="0.25">
@@ -6489,10 +7205,10 @@
         <v>68</v>
       </c>
       <c r="B81">
-        <v>132</v>
+        <v>71654</v>
       </c>
       <c r="C81">
-        <v>20541</v>
+        <v>20712</v>
       </c>
       <c r="D81">
         <f t="shared" si="1"/>
@@ -6504,14 +7220,14 @@
         <v>69</v>
       </c>
       <c r="B82">
-        <v>132</v>
+        <v>76664</v>
       </c>
       <c r="C82">
-        <v>20833</v>
+        <v>21005</v>
       </c>
       <c r="D82">
         <f t="shared" si="1"/>
-        <v>292</v>
+        <v>293</v>
       </c>
     </row>
     <row r="83" spans="1:4" x14ac:dyDescent="0.25">
@@ -6519,14 +7235,14 @@
         <v>70</v>
       </c>
       <c r="B83">
-        <v>132</v>
+        <v>73972</v>
       </c>
       <c r="C83">
-        <v>21124</v>
+        <v>21297</v>
       </c>
       <c r="D83">
         <f t="shared" si="1"/>
-        <v>291</v>
+        <v>292</v>
       </c>
     </row>
     <row r="84" spans="1:4" x14ac:dyDescent="0.25">
@@ -6534,14 +7250,14 @@
         <v>71</v>
       </c>
       <c r="B84">
-        <v>161</v>
+        <v>79104</v>
       </c>
       <c r="C84">
-        <v>21416</v>
+        <v>21590</v>
       </c>
       <c r="D84">
         <f t="shared" si="1"/>
-        <v>292</v>
+        <v>293</v>
       </c>
     </row>
     <row r="85" spans="1:4" x14ac:dyDescent="0.25">
@@ -6549,14 +7265,14 @@
         <v>72</v>
       </c>
       <c r="B85">
-        <v>132</v>
+        <v>76290</v>
       </c>
       <c r="C85">
-        <v>21708</v>
+        <v>21879</v>
       </c>
       <c r="D85">
         <f t="shared" si="1"/>
-        <v>292</v>
+        <v>289</v>
       </c>
     </row>
     <row r="86" spans="1:4" x14ac:dyDescent="0.25">
@@ -6564,14 +7280,14 @@
         <v>73</v>
       </c>
       <c r="B86">
-        <v>132</v>
+        <v>81544</v>
       </c>
       <c r="C86">
-        <v>22000</v>
+        <v>22172</v>
       </c>
       <c r="D86">
         <f t="shared" si="1"/>
-        <v>292</v>
+        <v>293</v>
       </c>
     </row>
     <row r="87" spans="1:4" x14ac:dyDescent="0.25">
@@ -6579,14 +7295,14 @@
         <v>74</v>
       </c>
       <c r="B87">
-        <v>132</v>
+        <v>78636</v>
       </c>
       <c r="C87">
-        <v>22292</v>
+        <v>22466</v>
       </c>
       <c r="D87">
         <f t="shared" si="1"/>
-        <v>292</v>
+        <v>294</v>
       </c>
     </row>
     <row r="88" spans="1:4" x14ac:dyDescent="0.25">
@@ -6594,14 +7310,14 @@
         <v>75</v>
       </c>
       <c r="B88">
-        <v>132</v>
+        <v>83984</v>
       </c>
       <c r="C88">
-        <v>22583</v>
+        <v>22758</v>
       </c>
       <c r="D88">
         <f t="shared" si="1"/>
-        <v>291</v>
+        <v>292</v>
       </c>
     </row>
     <row r="89" spans="1:4" x14ac:dyDescent="0.25">
@@ -6609,14 +7325,14 @@
         <v>76</v>
       </c>
       <c r="B89">
-        <v>103</v>
+        <v>80926</v>
       </c>
       <c r="C89">
-        <v>22874</v>
+        <v>23050</v>
       </c>
       <c r="D89">
         <f t="shared" si="1"/>
-        <v>291</v>
+        <v>292</v>
       </c>
     </row>
     <row r="90" spans="1:4" x14ac:dyDescent="0.25">
@@ -6624,14 +7340,14 @@
         <v>77</v>
       </c>
       <c r="B90">
-        <v>132</v>
+        <v>86424</v>
       </c>
       <c r="C90">
-        <v>23166</v>
+        <v>23341</v>
       </c>
       <c r="D90">
         <f t="shared" si="1"/>
-        <v>292</v>
+        <v>291</v>
       </c>
     </row>
     <row r="91" spans="1:4" x14ac:dyDescent="0.25">
@@ -6639,14 +7355,14 @@
         <v>78</v>
       </c>
       <c r="B91">
-        <v>132</v>
+        <v>83305</v>
       </c>
       <c r="C91">
-        <v>23457</v>
+        <v>23633</v>
       </c>
       <c r="D91">
         <f t="shared" si="1"/>
-        <v>291</v>
+        <v>292</v>
       </c>
     </row>
     <row r="92" spans="1:4" x14ac:dyDescent="0.25">
@@ -6654,14 +7370,14 @@
         <v>79</v>
       </c>
       <c r="B92">
-        <v>132</v>
+        <v>88864</v>
       </c>
       <c r="C92">
-        <v>23748</v>
+        <v>23926</v>
       </c>
       <c r="D92">
         <f t="shared" si="1"/>
-        <v>291</v>
+        <v>293</v>
       </c>
     </row>
     <row r="93" spans="1:4" x14ac:dyDescent="0.25">
@@ -6669,14 +7385,14 @@
         <v>80</v>
       </c>
       <c r="B93">
-        <v>132</v>
+        <v>85623</v>
       </c>
       <c r="C93">
-        <v>24039</v>
+        <v>24218</v>
       </c>
       <c r="D93">
         <f t="shared" si="1"/>
-        <v>291</v>
+        <v>292</v>
       </c>
     </row>
     <row r="94" spans="1:4" x14ac:dyDescent="0.25">
@@ -6684,14 +7400,14 @@
         <v>81</v>
       </c>
       <c r="B94">
-        <v>132</v>
+        <v>91304</v>
       </c>
       <c r="C94">
-        <v>24330</v>
+        <v>24510</v>
       </c>
       <c r="D94">
         <f t="shared" si="1"/>
-        <v>291</v>
+        <v>292</v>
       </c>
     </row>
     <row r="95" spans="1:4" x14ac:dyDescent="0.25">
@@ -6699,14 +7415,14 @@
         <v>82</v>
       </c>
       <c r="B95">
-        <v>161</v>
+        <v>87941</v>
       </c>
       <c r="C95">
-        <v>24621</v>
+        <v>24803</v>
       </c>
       <c r="D95">
         <f t="shared" si="1"/>
-        <v>291</v>
+        <v>293</v>
       </c>
     </row>
     <row r="96" spans="1:4" x14ac:dyDescent="0.25">
@@ -6714,10 +7430,10 @@
         <v>83</v>
       </c>
       <c r="B96">
-        <v>103</v>
+        <v>93744</v>
       </c>
       <c r="C96">
-        <v>24913</v>
+        <v>25095</v>
       </c>
       <c r="D96">
         <f t="shared" si="1"/>
@@ -6729,10 +7445,10 @@
         <v>84</v>
       </c>
       <c r="B97">
-        <v>132</v>
+        <v>90259</v>
       </c>
       <c r="C97">
-        <v>25205</v>
+        <v>25387</v>
       </c>
       <c r="D97">
         <f t="shared" si="1"/>
@@ -6744,14 +7460,14 @@
         <v>85</v>
       </c>
       <c r="B98">
-        <v>132</v>
+        <v>96184</v>
       </c>
       <c r="C98">
-        <v>25496</v>
+        <v>25681</v>
       </c>
       <c r="D98">
         <f t="shared" si="1"/>
-        <v>291</v>
+        <v>294</v>
       </c>
     </row>
     <row r="99" spans="1:4" x14ac:dyDescent="0.25">
@@ -6759,14 +7475,14 @@
         <v>86</v>
       </c>
       <c r="B99">
-        <v>132</v>
+        <v>92577</v>
       </c>
       <c r="C99">
-        <v>25787</v>
+        <v>25973</v>
       </c>
       <c r="D99">
         <f t="shared" si="1"/>
-        <v>291</v>
+        <v>292</v>
       </c>
     </row>
     <row r="100" spans="1:4" x14ac:dyDescent="0.25">
@@ -6774,14 +7490,14 @@
         <v>87</v>
       </c>
       <c r="B100">
-        <v>161</v>
+        <v>93675</v>
       </c>
       <c r="C100">
-        <v>26080</v>
+        <v>26264</v>
       </c>
       <c r="D100">
         <f t="shared" si="1"/>
-        <v>293</v>
+        <v>291</v>
       </c>
     </row>
     <row r="101" spans="1:4" x14ac:dyDescent="0.25">
@@ -6789,14 +7505,14 @@
         <v>88</v>
       </c>
       <c r="B101">
-        <v>132</v>
+        <v>99844</v>
       </c>
       <c r="C101">
-        <v>26370</v>
+        <v>26555</v>
       </c>
       <c r="D101">
         <f t="shared" si="1"/>
-        <v>290</v>
+        <v>291</v>
       </c>
     </row>
     <row r="102" spans="1:4" x14ac:dyDescent="0.25">
@@ -6804,14 +7520,14 @@
         <v>89</v>
       </c>
       <c r="B102">
-        <v>103</v>
+        <v>95993</v>
       </c>
       <c r="C102">
-        <v>26661</v>
+        <v>26847</v>
       </c>
       <c r="D102">
         <f t="shared" si="1"/>
-        <v>291</v>
+        <v>292</v>
       </c>
     </row>
     <row r="103" spans="1:4" x14ac:dyDescent="0.25">
@@ -6819,14 +7535,14 @@
         <v>90</v>
       </c>
       <c r="B103">
-        <v>132</v>
+        <v>102284</v>
       </c>
       <c r="C103">
-        <v>26952</v>
+        <v>27139</v>
       </c>
       <c r="D103">
         <f t="shared" si="1"/>
-        <v>291</v>
+        <v>292</v>
       </c>
     </row>
     <row r="104" spans="1:4" x14ac:dyDescent="0.25">
@@ -6834,10 +7550,10 @@
         <v>91</v>
       </c>
       <c r="B104">
-        <v>132</v>
+        <v>98311</v>
       </c>
       <c r="C104">
-        <v>27243</v>
+        <v>27430</v>
       </c>
       <c r="D104">
         <f t="shared" si="1"/>
@@ -6849,14 +7565,14 @@
         <v>92</v>
       </c>
       <c r="B105">
-        <v>128</v>
+        <v>104724</v>
       </c>
       <c r="C105">
-        <v>27534</v>
+        <v>27723</v>
       </c>
       <c r="D105">
         <f t="shared" si="1"/>
-        <v>291</v>
+        <v>293</v>
       </c>
     </row>
     <row r="106" spans="1:4" x14ac:dyDescent="0.25">
@@ -6864,14 +7580,14 @@
         <v>93</v>
       </c>
       <c r="B106">
-        <v>132</v>
+        <v>100641</v>
       </c>
       <c r="C106">
-        <v>27825</v>
+        <v>28015</v>
       </c>
       <c r="D106">
         <f t="shared" si="1"/>
-        <v>291</v>
+        <v>292</v>
       </c>
     </row>
     <row r="107" spans="1:4" x14ac:dyDescent="0.25">
@@ -6879,10 +7595,10 @@
         <v>94</v>
       </c>
       <c r="B107">
-        <v>132</v>
+        <v>107164</v>
       </c>
       <c r="C107">
-        <v>28116</v>
+        <v>28306</v>
       </c>
       <c r="D107">
         <f t="shared" si="1"/>
@@ -6894,14 +7610,14 @@
         <v>95</v>
       </c>
       <c r="B108">
-        <v>132</v>
+        <v>103008</v>
       </c>
       <c r="C108">
-        <v>28407</v>
+        <v>28598</v>
       </c>
       <c r="D108">
         <f t="shared" si="1"/>
-        <v>291</v>
+        <v>292</v>
       </c>
     </row>
     <row r="109" spans="1:4" x14ac:dyDescent="0.25">
@@ -6909,10 +7625,10 @@
         <v>96</v>
       </c>
       <c r="B109">
-        <v>103</v>
+        <v>104106</v>
       </c>
       <c r="C109">
-        <v>28698</v>
+        <v>28889</v>
       </c>
       <c r="D109">
         <f t="shared" si="1"/>
@@ -6924,14 +7640,14 @@
         <v>97</v>
       </c>
       <c r="B110">
-        <v>132</v>
+        <v>110824</v>
       </c>
       <c r="C110">
-        <v>28990</v>
+        <v>29182</v>
       </c>
       <c r="D110">
         <f t="shared" si="1"/>
-        <v>292</v>
+        <v>293</v>
       </c>
     </row>
     <row r="111" spans="1:4" x14ac:dyDescent="0.25">
@@ -6939,14 +7655,14 @@
         <v>98</v>
       </c>
       <c r="B111">
-        <v>132</v>
+        <v>112044</v>
       </c>
       <c r="C111">
-        <v>29282</v>
+        <v>29476</v>
       </c>
       <c r="D111">
         <f t="shared" si="1"/>
-        <v>292</v>
+        <v>294</v>
       </c>
     </row>
     <row r="112" spans="1:4" x14ac:dyDescent="0.25">
@@ -6954,14 +7670,14 @@
         <v>99</v>
       </c>
       <c r="B112">
-        <v>132</v>
+        <v>107644</v>
       </c>
       <c r="C112">
-        <v>29573</v>
+        <v>29768</v>
       </c>
       <c r="D112">
         <f t="shared" si="1"/>
-        <v>291</v>
+        <v>292</v>
       </c>
     </row>
     <row r="113" spans="1:4" x14ac:dyDescent="0.25">
@@ -6969,14 +7685,14 @@
         <v>100</v>
       </c>
       <c r="B113">
-        <v>132</v>
+        <v>108742</v>
       </c>
       <c r="C113">
-        <v>29864</v>
+        <v>30060</v>
       </c>
       <c r="D113">
         <f t="shared" si="1"/>
-        <v>291</v>
+        <v>292</v>
       </c>
     </row>
     <row r="114" spans="1:4" x14ac:dyDescent="0.25">
@@ -6984,14 +7700,14 @@
         <v>101</v>
       </c>
       <c r="B114">
-        <v>132</v>
+        <v>115704</v>
       </c>
       <c r="C114">
-        <v>30156</v>
+        <v>30351</v>
       </c>
       <c r="D114">
         <f t="shared" si="1"/>
-        <v>292</v>
+        <v>291</v>
       </c>
     </row>
     <row r="115" spans="1:4" x14ac:dyDescent="0.25">
@@ -6999,14 +7715,14 @@
         <v>102</v>
       </c>
       <c r="B115">
-        <v>132</v>
+        <v>111060</v>
       </c>
       <c r="C115">
-        <v>30449</v>
+        <v>30643</v>
       </c>
       <c r="D115">
         <f t="shared" si="1"/>
-        <v>293</v>
+        <v>292</v>
       </c>
     </row>
     <row r="116" spans="1:4" x14ac:dyDescent="0.25">
@@ -7014,14 +7730,14 @@
         <v>103</v>
       </c>
       <c r="B116">
-        <v>161</v>
+        <v>117616</v>
       </c>
       <c r="C116">
-        <v>30740</v>
+        <v>30935</v>
       </c>
       <c r="D116">
         <f t="shared" si="1"/>
-        <v>291</v>
+        <v>292</v>
       </c>
     </row>
     <row r="117" spans="1:4" x14ac:dyDescent="0.25">
@@ -7029,14 +7745,14 @@
         <v>104</v>
       </c>
       <c r="B117">
-        <v>132</v>
+        <v>112256</v>
       </c>
       <c r="C117">
-        <v>31032</v>
+        <v>31226</v>
       </c>
       <c r="D117">
         <f t="shared" si="1"/>
-        <v>292</v>
+        <v>291</v>
       </c>
     </row>
     <row r="118" spans="1:4" x14ac:dyDescent="0.25">
@@ -7044,10 +7760,10 @@
         <v>105</v>
       </c>
       <c r="B118">
-        <v>136</v>
+        <v>118736</v>
       </c>
       <c r="C118">
-        <v>31324</v>
+        <v>31518</v>
       </c>
       <c r="D118">
         <f t="shared" si="1"/>
@@ -7059,14 +7775,14 @@
         <v>106</v>
       </c>
       <c r="B119">
-        <v>132</v>
+        <v>113348</v>
       </c>
       <c r="C119">
-        <v>31615</v>
+        <v>31811</v>
       </c>
       <c r="D119">
         <f t="shared" si="1"/>
-        <v>291</v>
+        <v>293</v>
       </c>
     </row>
     <row r="120" spans="1:4" x14ac:dyDescent="0.25">
@@ -7074,10 +7790,10 @@
         <v>107</v>
       </c>
       <c r="B120">
-        <v>128</v>
+        <v>119856</v>
       </c>
       <c r="C120">
-        <v>31907</v>
+        <v>32103</v>
       </c>
       <c r="D120">
         <f t="shared" si="1"/>
@@ -7089,14 +7805,14 @@
         <v>108</v>
       </c>
       <c r="B121">
-        <v>132</v>
+        <v>114412</v>
       </c>
       <c r="C121">
-        <v>32197</v>
+        <v>32394</v>
       </c>
       <c r="D121">
         <f t="shared" si="1"/>
-        <v>290</v>
+        <v>291</v>
       </c>
     </row>
     <row r="122" spans="1:4" x14ac:dyDescent="0.25">
@@ -7104,10 +7820,10 @@
         <v>109</v>
       </c>
       <c r="B122">
-        <v>132</v>
+        <v>120784</v>
       </c>
       <c r="C122">
-        <v>32489</v>
+        <v>32686</v>
       </c>
       <c r="D122">
         <f t="shared" si="1"/>
@@ -7119,14 +7835,14 @@
         <v>110</v>
       </c>
       <c r="B123">
-        <v>33</v>
+        <v>114980</v>
       </c>
       <c r="C123">
-        <v>32781</v>
+        <v>32977</v>
       </c>
       <c r="D123">
         <f t="shared" si="1"/>
-        <v>292</v>
+        <v>291</v>
       </c>
     </row>
     <row r="124" spans="1:4" x14ac:dyDescent="0.25">
@@ -7134,14 +7850,14 @@
         <v>111</v>
       </c>
       <c r="B124">
-        <v>0</v>
+        <v>115196</v>
       </c>
       <c r="C124">
-        <v>33071</v>
+        <v>33269</v>
       </c>
       <c r="D124">
         <f t="shared" si="1"/>
-        <v>290</v>
+        <v>292</v>
       </c>
     </row>
     <row r="125" spans="1:4" x14ac:dyDescent="0.25">
@@ -7149,14 +7865,14 @@
         <v>112</v>
       </c>
       <c r="B125">
-        <v>0</v>
+        <v>121504</v>
       </c>
       <c r="C125">
-        <v>33361</v>
+        <v>33561</v>
       </c>
       <c r="D125">
         <f t="shared" si="1"/>
-        <v>290</v>
+        <v>292</v>
       </c>
     </row>
     <row r="126" spans="1:4" x14ac:dyDescent="0.25">
@@ -7164,14 +7880,14 @@
         <v>113</v>
       </c>
       <c r="B126">
-        <v>0</v>
+        <v>115652</v>
       </c>
       <c r="C126">
-        <v>33652</v>
+        <v>33854</v>
       </c>
       <c r="D126">
         <f t="shared" si="1"/>
-        <v>291</v>
+        <v>293</v>
       </c>
     </row>
     <row r="127" spans="1:4" x14ac:dyDescent="0.25">
@@ -7179,14 +7895,14 @@
         <v>114</v>
       </c>
       <c r="B127">
-        <v>0</v>
+        <v>121984</v>
       </c>
       <c r="C127">
-        <v>33944</v>
+        <v>34144</v>
       </c>
       <c r="D127">
         <f t="shared" si="1"/>
-        <v>292</v>
+        <v>290</v>
       </c>
     </row>
     <row r="128" spans="1:4" x14ac:dyDescent="0.25">
@@ -7194,14 +7910,14 @@
         <v>115</v>
       </c>
       <c r="B128">
-        <v>0</v>
+        <v>115976</v>
       </c>
       <c r="C128">
-        <v>34234</v>
+        <v>34435</v>
       </c>
       <c r="D128">
         <f t="shared" si="1"/>
-        <v>290</v>
+        <v>291</v>
       </c>
     </row>
     <row r="129" spans="1:4" x14ac:dyDescent="0.25">
@@ -7209,14 +7925,14 @@
         <v>116</v>
       </c>
       <c r="B129">
-        <v>0</v>
+        <v>122080</v>
       </c>
       <c r="C129">
-        <v>34525</v>
+        <v>34727</v>
       </c>
       <c r="D129">
         <f t="shared" si="1"/>
-        <v>291</v>
+        <v>292</v>
       </c>
     </row>
     <row r="130" spans="1:4" x14ac:dyDescent="0.25">
@@ -7224,14 +7940,14 @@
         <v>117</v>
       </c>
       <c r="B130">
-        <v>0</v>
+        <v>115976</v>
       </c>
       <c r="C130">
-        <v>34817</v>
+        <v>35018</v>
       </c>
       <c r="D130">
         <f t="shared" si="1"/>
-        <v>292</v>
+        <v>291</v>
       </c>
     </row>
     <row r="131" spans="1:4" x14ac:dyDescent="0.25">
@@ -7239,14 +7955,14 @@
         <v>118</v>
       </c>
       <c r="B131">
-        <v>0</v>
+        <v>122080</v>
       </c>
       <c r="C131">
-        <v>35107</v>
+        <v>35311</v>
       </c>
       <c r="D131">
         <f t="shared" si="1"/>
-        <v>290</v>
+        <v>293</v>
       </c>
     </row>
     <row r="132" spans="1:4" x14ac:dyDescent="0.25">
@@ -7254,14 +7970,14 @@
         <v>119</v>
       </c>
       <c r="B132">
-        <v>0</v>
+        <v>115976</v>
       </c>
       <c r="C132">
-        <v>35398</v>
+        <v>35603</v>
       </c>
       <c r="D132">
         <f t="shared" si="1"/>
-        <v>291</v>
+        <v>292</v>
       </c>
     </row>
     <row r="133" spans="1:4" x14ac:dyDescent="0.25">
@@ -7269,14 +7985,14 @@
         <v>120</v>
       </c>
       <c r="B133">
-        <v>0</v>
+        <v>115976</v>
       </c>
       <c r="C133">
-        <v>35689</v>
+        <v>35895</v>
       </c>
       <c r="D133">
         <f t="shared" si="1"/>
-        <v>291</v>
+        <v>292</v>
       </c>
     </row>
     <row r="134" spans="1:4" x14ac:dyDescent="0.25">
@@ -7284,14 +8000,14 @@
         <v>121</v>
       </c>
       <c r="B134">
-        <v>0</v>
+        <v>122080</v>
       </c>
       <c r="C134">
-        <v>35980</v>
+        <v>36187</v>
       </c>
       <c r="D134">
         <f t="shared" si="1"/>
-        <v>291</v>
+        <v>292</v>
       </c>
     </row>
     <row r="135" spans="1:4" x14ac:dyDescent="0.25">
@@ -7299,14 +8015,14 @@
         <v>122</v>
       </c>
       <c r="B135">
-        <v>0</v>
+        <v>115976</v>
       </c>
       <c r="C135">
-        <v>36271</v>
+        <v>36479</v>
       </c>
       <c r="D135">
         <f t="shared" si="1"/>
-        <v>291</v>
+        <v>292</v>
       </c>
     </row>
     <row r="136" spans="1:4" x14ac:dyDescent="0.25">
@@ -7317,11 +8033,11 @@
         <v>0</v>
       </c>
       <c r="C136">
-        <v>36561</v>
+        <v>37054</v>
       </c>
       <c r="D136">
         <f t="shared" si="1"/>
-        <v>290</v>
+        <v>575</v>
       </c>
     </row>
     <row r="137" spans="1:4" x14ac:dyDescent="0.25">
@@ -7332,11 +8048,11 @@
         <v>0</v>
       </c>
       <c r="C137">
-        <v>36851</v>
+        <v>37346</v>
       </c>
       <c r="D137">
         <f t="shared" si="1"/>
-        <v>290</v>
+        <v>292</v>
       </c>
     </row>
     <row r="138" spans="1:4" x14ac:dyDescent="0.25">
@@ -7347,11 +8063,11 @@
         <v>0</v>
       </c>
       <c r="C138">
-        <v>37143</v>
+        <v>37639</v>
       </c>
       <c r="D138">
         <f t="shared" si="1"/>
-        <v>292</v>
+        <v>293</v>
       </c>
     </row>
     <row r="139" spans="1:4" x14ac:dyDescent="0.25">
@@ -7362,11 +8078,11 @@
         <v>0</v>
       </c>
       <c r="C139">
-        <v>37434</v>
+        <v>37931</v>
       </c>
       <c r="D139">
         <f t="shared" si="1"/>
-        <v>291</v>
+        <v>292</v>
       </c>
     </row>
     <row r="140" spans="1:4" x14ac:dyDescent="0.25">
@@ -7377,149 +8093,62 @@
         <v>0</v>
       </c>
       <c r="C140">
-        <v>37726</v>
+        <v>38214</v>
       </c>
       <c r="D140">
-        <f t="shared" ref="D140:D149" si="2">C140-C139</f>
-        <v>292</v>
+        <f t="shared" ref="D140" si="2">C140-C139</f>
+        <v>283</v>
       </c>
     </row>
     <row r="141" spans="1:4" x14ac:dyDescent="0.25">
       <c r="A141">
         <v>128</v>
       </c>
-      <c r="B141">
-        <v>0</v>
-      </c>
-      <c r="C141">
-        <v>38018</v>
-      </c>
-      <c r="D141">
-        <f t="shared" si="2"/>
-        <v>292</v>
-      </c>
     </row>
     <row r="142" spans="1:4" x14ac:dyDescent="0.25">
       <c r="A142">
         <v>129</v>
       </c>
-      <c r="B142">
-        <v>0</v>
-      </c>
-      <c r="C142">
-        <v>38308</v>
-      </c>
-      <c r="D142">
-        <f t="shared" si="2"/>
-        <v>290</v>
-      </c>
     </row>
     <row r="143" spans="1:4" x14ac:dyDescent="0.25">
       <c r="A143">
         <v>130</v>
       </c>
-      <c r="B143">
-        <v>0</v>
-      </c>
-      <c r="C143">
-        <v>38599</v>
-      </c>
-      <c r="D143">
-        <f t="shared" si="2"/>
-        <v>291</v>
-      </c>
     </row>
     <row r="144" spans="1:4" x14ac:dyDescent="0.25">
       <c r="A144">
         <v>131</v>
       </c>
-      <c r="B144">
-        <v>0</v>
-      </c>
-      <c r="C144">
-        <v>38942</v>
-      </c>
-      <c r="D144">
-        <f t="shared" si="2"/>
-        <v>343</v>
-      </c>
-    </row>
-    <row r="145" spans="1:4" x14ac:dyDescent="0.25">
+    </row>
+    <row r="145" spans="1:1" x14ac:dyDescent="0.25">
       <c r="A145">
         <v>132</v>
       </c>
-      <c r="B145">
-        <v>0</v>
-      </c>
-      <c r="C145">
-        <v>39233</v>
-      </c>
-      <c r="D145">
-        <f t="shared" si="2"/>
-        <v>291</v>
-      </c>
-    </row>
-    <row r="146" spans="1:4" x14ac:dyDescent="0.25">
+    </row>
+    <row r="146" spans="1:1" x14ac:dyDescent="0.25">
       <c r="A146">
         <v>133</v>
       </c>
-      <c r="B146">
-        <v>0</v>
-      </c>
-      <c r="C146">
-        <v>39525</v>
-      </c>
-      <c r="D146">
-        <f>C146-C145</f>
-        <v>292</v>
-      </c>
-    </row>
-    <row r="147" spans="1:4" x14ac:dyDescent="0.25">
+    </row>
+    <row r="147" spans="1:1" x14ac:dyDescent="0.25">
       <c r="A147">
         <v>134</v>
       </c>
-      <c r="B147">
-        <v>0</v>
-      </c>
-      <c r="C147">
-        <v>39815</v>
-      </c>
-      <c r="D147">
-        <f t="shared" si="2"/>
-        <v>290</v>
-      </c>
-    </row>
-    <row r="148" spans="1:4" x14ac:dyDescent="0.25">
+    </row>
+    <row r="148" spans="1:1" x14ac:dyDescent="0.25">
       <c r="A148">
         <v>135</v>
       </c>
-      <c r="B148">
-        <v>0</v>
-      </c>
-      <c r="C148">
-        <v>40083</v>
-      </c>
-      <c r="D148">
-        <f t="shared" si="2"/>
-        <v>268</v>
-      </c>
-    </row>
-    <row r="149" spans="1:4" x14ac:dyDescent="0.25">
+    </row>
+    <row r="149" spans="1:1" x14ac:dyDescent="0.25">
       <c r="A149">
         <v>136</v>
       </c>
-      <c r="B149">
-        <v>0</v>
-      </c>
-      <c r="C149">
-        <v>40376</v>
-      </c>
-      <c r="D149">
-        <f>C149-C148</f>
-        <v>293</v>
-      </c>
     </row>
   </sheetData>
+  <mergeCells count="1">
+    <mergeCell ref="B1:D1"/>
+  </mergeCells>
   <pageMargins left="0.7" right="0.7" top="0.75" bottom="0.75" header="0.3" footer="0.3"/>
 </worksheet>
 </file>
</xml_diff>